<commit_message>
cleaned code, added back-casting functionality
</commit_message>
<xml_diff>
--- a/data/reg_input/Development Test Data Regression Inputs.xlsx
+++ b/data/reg_input/Development Test Data Regression Inputs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fidias\Coding-related\Python\Traffic-Regression-Tool\data\reg_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6421EA2-8A77-4E86-8364-8B3CF57F0FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC20670-9E83-4C1B-B64C-8B9F7256498F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9130" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30840" yWindow="-120" windowWidth="30030" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="74">
   <si>
     <t>Confidential</t>
   </si>
@@ -261,13 +261,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0;[Red]\(#,##0\);\-"/>
     <numFmt numFmtId="165" formatCode="[Red]&quot;E: &quot;#,##0;[Red]&quot;E: &quot;\-#,##0;[Blue]&quot;OK&quot;"/>
     <numFmt numFmtId="166" formatCode="#,##0.0%;[Red]\(#,##0.0%\);\-"/>
     <numFmt numFmtId="167" formatCode="#,##0;\(#,##0\);\-"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -447,6 +448,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -729,7 +736,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0">
       <alignment vertical="center"/>
@@ -853,8 +860,9 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="13"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="14"/>
+    <xf numFmtId="43" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -883,8 +891,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="51" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="5" borderId="2" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="52">
     <cellStyle name="A1.Title1" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="A1.Title2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="A2.Heading1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -917,6 +929,7 @@
     <cellStyle name="C2.totalpercentage" xfId="32" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="Calculation" xfId="44" builtinId="22" hidden="1"/>
     <cellStyle name="Check Cell" xfId="46" builtinId="23" hidden="1"/>
+    <cellStyle name="Comma" xfId="51" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="49" builtinId="53" hidden="1"/>
     <cellStyle name="Heading 1" xfId="38" builtinId="16" hidden="1"/>
     <cellStyle name="Heading 2" xfId="39" builtinId="17" hidden="1"/>
@@ -1251,10 +1264,10 @@
     <tabColor theme="6" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BO40"/>
+  <dimension ref="B2:BO47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1262,7 +1275,9 @@
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="3" width="9.09765625" customWidth="1"/>
     <col min="4" max="4" width="19.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="19" width="9.09765625" customWidth="1"/>
+    <col min="5" max="9" width="9.09765625" customWidth="1"/>
+    <col min="10" max="10" width="7.796875" customWidth="1"/>
+    <col min="11" max="19" width="9.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3843,15 +3858,15 @@
         <v>0</v>
       </c>
       <c r="R28" s="8">
-        <v>0</v>
-      </c>
-      <c r="S28" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="S28" s="11">
         <v>0.5</v>
       </c>
-      <c r="T28" s="8">
+      <c r="T28" s="11">
         <v>0.75</v>
       </c>
-      <c r="U28" s="8">
+      <c r="U28" s="11">
         <v>1</v>
       </c>
       <c r="V28" s="8">
@@ -4256,6 +4271,1092 @@
       </c>
       <c r="BB30" s="8">
         <v>148.21550411007593</v>
+      </c>
+    </row>
+    <row r="32" spans="4:54" x14ac:dyDescent="0.3">
+      <c r="J32" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K32" s="10">
+        <f>(K25/G25)</f>
+        <v>0.96395632100181672</v>
+      </c>
+      <c r="L32" s="10">
+        <f t="shared" ref="L32:BB32" si="0">(L25/H25)</f>
+        <v>0.98453838433411589</v>
+      </c>
+      <c r="M32" s="10">
+        <f t="shared" si="0"/>
+        <v>0.99439894284238561</v>
+      </c>
+      <c r="N32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.021430405139844</v>
+      </c>
+      <c r="O32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0106696832579185</v>
+      </c>
+      <c r="P32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0063994323591228</v>
+      </c>
+      <c r="Q32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0087580835199625</v>
+      </c>
+      <c r="R32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0059029986521413</v>
+      </c>
+      <c r="S32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0189292525900124</v>
+      </c>
+      <c r="T32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.018574214305157</v>
+      </c>
+      <c r="U32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.018766146486948</v>
+      </c>
+      <c r="V32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0154359477817874</v>
+      </c>
+      <c r="W32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0136388002776973</v>
+      </c>
+      <c r="X32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0136596521125805</v>
+      </c>
+      <c r="Y32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0243957938588237</v>
+      </c>
+      <c r="Z32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0290089866452399</v>
+      </c>
+      <c r="AA32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.036221769474186</v>
+      </c>
+      <c r="AB32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0383457623016534</v>
+      </c>
+      <c r="AC32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0334283078027151</v>
+      </c>
+      <c r="AD32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0323388190680951</v>
+      </c>
+      <c r="AE32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0278126385716557</v>
+      </c>
+      <c r="AF32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0306175963771675</v>
+      </c>
+      <c r="AG32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0288851641117958</v>
+      </c>
+      <c r="AH32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0266767245885442</v>
+      </c>
+      <c r="AI32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0281141824501565</v>
+      </c>
+      <c r="AJ32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0261479746375348</v>
+      </c>
+      <c r="AK32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0253845242184472</v>
+      </c>
+      <c r="AL32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0276746763035209</v>
+      </c>
+      <c r="AM32" s="10">
+        <f t="shared" si="0"/>
+        <v>0.97421041796977059</v>
+      </c>
+      <c r="AN32" s="10">
+        <f t="shared" si="0"/>
+        <v>0.82220481768860365</v>
+      </c>
+      <c r="AO32" s="10">
+        <f t="shared" si="0"/>
+        <v>0.93804215805352043</v>
+      </c>
+      <c r="AP32" s="10">
+        <f t="shared" si="0"/>
+        <v>0.93354782054569896</v>
+      </c>
+      <c r="AQ32" s="10">
+        <f t="shared" si="0"/>
+        <v>0.95252704830598878</v>
+      </c>
+      <c r="AR32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.1719787754984814</v>
+      </c>
+      <c r="AS32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0531417007599726</v>
+      </c>
+      <c r="AT32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0693322955514117</v>
+      </c>
+      <c r="AU32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.1213434013779568</v>
+      </c>
+      <c r="AV32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.074175728799714</v>
+      </c>
+      <c r="AW32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0481915764884122</v>
+      </c>
+      <c r="AX32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0339433311211752</v>
+      </c>
+      <c r="AY32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0254119768611958</v>
+      </c>
+      <c r="AZ32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0251940600421676</v>
+      </c>
+      <c r="BA32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="BB32" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0209999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:67" x14ac:dyDescent="0.3">
+      <c r="J33" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K33" s="10">
+        <f>EXP(K26-G26)</f>
+        <v>16.444646771097062</v>
+      </c>
+      <c r="L33" s="10">
+        <f>EXP(L26-H26)</f>
+        <v>4.9530324243951043</v>
+      </c>
+      <c r="M33" s="10">
+        <f>EXP(M26-I26)</f>
+        <v>0.74081822068171732</v>
+      </c>
+      <c r="N33" s="10">
+        <f>EXP(N26-J26)</f>
+        <v>0.18268352405273477</v>
+      </c>
+      <c r="O33" s="10">
+        <f>EXP(O26-K26)</f>
+        <v>6.7205512739749812E-2</v>
+      </c>
+      <c r="P33" s="10">
+        <f>EXP(P26-L26)</f>
+        <v>6.0810062625218028E-2</v>
+      </c>
+      <c r="Q33" s="10">
+        <f>EXP(Q26-M26)</f>
+        <v>6.7205512739749687E-2</v>
+      </c>
+      <c r="R33" s="10">
+        <f>EXP(R26-N26)</f>
+        <v>0.12245642825298195</v>
+      </c>
+      <c r="S33" s="10">
+        <f>EXP(S26-O26)</f>
+        <v>0.22313016014842982</v>
+      </c>
+      <c r="T33" s="10">
+        <f>EXP(T26-P26)</f>
+        <v>0.11080315836233397</v>
+      </c>
+      <c r="U33" s="10">
+        <f>EXP(U26-Q26)</f>
+        <v>0.27253179303401337</v>
+      </c>
+      <c r="V33" s="10">
+        <f>EXP(V26-R26)</f>
+        <v>0.27253179303401193</v>
+      </c>
+      <c r="W33" s="10">
+        <f>EXP(W26-S26)</f>
+        <v>0.22313016014842982</v>
+      </c>
+      <c r="X33" s="10">
+        <f>EXP(X26-T26)</f>
+        <v>0.30119421191220175</v>
+      </c>
+      <c r="Y33" s="10">
+        <f>EXP(Y26-U26)</f>
+        <v>0.22313016014842982</v>
+      </c>
+      <c r="Z33" s="10">
+        <f>EXP(Z26-V26)</f>
+        <v>0.14956861922263526</v>
+      </c>
+      <c r="AA33" s="10">
+        <f>EXP(AA26-W26)</f>
+        <v>9.071795328941247E-2</v>
+      </c>
+      <c r="AB33" s="10">
+        <f>EXP(AB26-X26)</f>
+        <v>0.1353352832366127</v>
+      </c>
+      <c r="AC33" s="10">
+        <f>EXP(AC26-Y26)</f>
+        <v>0.11080315836233376</v>
+      </c>
+      <c r="AD33" s="10">
+        <f>EXP(AD26-Z26)</f>
+        <v>8.20849986238988E-2</v>
+      </c>
+      <c r="AE33" s="10">
+        <f>EXP(AE26-AA26)</f>
+        <v>0.10025884372280366</v>
+      </c>
+      <c r="AF33" s="10">
+        <f>EXP(AF26-AB26)</f>
+        <v>0.10025884372280384</v>
+      </c>
+      <c r="AG33" s="10">
+        <f>EXP(AG26-AC26)</f>
+        <v>0.16529888822158673</v>
+      </c>
+      <c r="AH33" s="10">
+        <f>EXP(AH26-AD26)</f>
+        <v>0.22313016014842982</v>
+      </c>
+      <c r="AI33" s="10">
+        <f>EXP(AI26-AE26)</f>
+        <v>0.3011942119122023</v>
+      </c>
+      <c r="AJ33" s="10">
+        <f>EXP(AJ26-AF26)</f>
+        <v>0.60653065971263342</v>
+      </c>
+      <c r="AK33" s="10">
+        <f>EXP(AK26-AG26)</f>
+        <v>0.54881163609402617</v>
+      </c>
+      <c r="AL33" s="10">
+        <f>EXP(AL26-AH26)</f>
+        <v>1.1051709180756473</v>
+      </c>
+      <c r="AM33" s="10">
+        <f>EXP(AM26-AI26)</f>
+        <v>0.90483741803595985</v>
+      </c>
+      <c r="AN33" s="10">
+        <f>EXP(AN26-AJ26)</f>
+        <v>0.49658530379140942</v>
+      </c>
+      <c r="AO33" s="10">
+        <f>EXP(AO26-AK26)</f>
+        <v>5.4739473917272008</v>
+      </c>
+      <c r="AP33" s="10">
+        <f>EXP(AP26-AL26)</f>
+        <v>1.4918246976412695</v>
+      </c>
+      <c r="AQ33" s="10">
+        <f>EXP(AQ26-AM26)</f>
+        <v>1.3498588075760016</v>
+      </c>
+      <c r="AR33" s="10">
+        <f>EXP(AR26-AN26)</f>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="AS33" s="10">
+        <f>EXP(AS26-AO26)</f>
+        <v>0.14956861922263501</v>
+      </c>
+      <c r="AT33" s="10">
+        <f>EXP(AT26-AP26)</f>
+        <v>0.36787944117144233</v>
+      </c>
+      <c r="AU33" s="10">
+        <f>EXP(AU26-AQ26)</f>
+        <v>0.3011942119122023</v>
+      </c>
+      <c r="AV33" s="10">
+        <f>EXP(AV26-AR26)</f>
+        <v>0.36787944117144233</v>
+      </c>
+      <c r="AW33" s="10">
+        <f>EXP(AW26-AS26)</f>
+        <v>0.74081822068171799</v>
+      </c>
+      <c r="AX33" s="10">
+        <f>EXP(AX26-AT26)</f>
+        <v>1.2214027581601701</v>
+      </c>
+      <c r="AY33" s="10">
+        <f>EXP(AY26-AU26)</f>
+        <v>3.6692966676192467</v>
+      </c>
+      <c r="AZ33" s="10">
+        <f>EXP(AZ26-AV26)</f>
+        <v>1.4918246976412695</v>
+      </c>
+      <c r="BA33" s="10">
+        <f>EXP(BA26-AW26)</f>
+        <v>2.2255409284924692</v>
+      </c>
+      <c r="BB33" s="10">
+        <f>EXP(BB26-AX26)</f>
+        <v>1.1051709180756482</v>
+      </c>
+    </row>
+    <row r="34" spans="2:67" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J34" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="10">
+        <f>EXP(K27-G27)</f>
+        <v>1</v>
+      </c>
+      <c r="L34" s="10">
+        <f>EXP(L27-H27)</f>
+        <v>1</v>
+      </c>
+      <c r="M34" s="10">
+        <f>EXP(M27-I27)</f>
+        <v>1</v>
+      </c>
+      <c r="N34" s="10">
+        <f>EXP(N27-J27)</f>
+        <v>1</v>
+      </c>
+      <c r="O34" s="10">
+        <f>EXP(O27-K27)</f>
+        <v>1</v>
+      </c>
+      <c r="P34" s="10">
+        <f>EXP(P27-L27)</f>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="Q34" s="10">
+        <f>EXP(Q27-M27)</f>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="R34" s="10">
+        <f>EXP(R27-N27)</f>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="S34" s="10">
+        <f>EXP(S27-O27)</f>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="T34" s="10">
+        <f>EXP(T27-P27)</f>
+        <v>1</v>
+      </c>
+      <c r="U34" s="10">
+        <f>EXP(U27-Q27)</f>
+        <v>1</v>
+      </c>
+      <c r="V34" s="10">
+        <f>EXP(V27-R27)</f>
+        <v>1</v>
+      </c>
+      <c r="W34" s="10">
+        <f>EXP(W27-S27)</f>
+        <v>1</v>
+      </c>
+      <c r="X34" s="10">
+        <f>EXP(X27-T27)</f>
+        <v>1</v>
+      </c>
+      <c r="Y34" s="10">
+        <f>EXP(Y27-U27)</f>
+        <v>1</v>
+      </c>
+      <c r="Z34" s="10">
+        <f>EXP(Z27-V27)</f>
+        <v>1</v>
+      </c>
+      <c r="AA34" s="10">
+        <f>EXP(AA27-W27)</f>
+        <v>1</v>
+      </c>
+      <c r="AB34" s="10">
+        <f>EXP(AB27-X27)</f>
+        <v>1</v>
+      </c>
+      <c r="AC34" s="10">
+        <f>EXP(AC27-Y27)</f>
+        <v>1</v>
+      </c>
+      <c r="AD34" s="10">
+        <f>EXP(AD27-Z27)</f>
+        <v>1</v>
+      </c>
+      <c r="AE34" s="10">
+        <f>EXP(AE27-AA27)</f>
+        <v>1</v>
+      </c>
+      <c r="AF34" s="10">
+        <f>EXP(AF27-AB27)</f>
+        <v>1</v>
+      </c>
+      <c r="AG34" s="10">
+        <f>EXP(AG27-AC27)</f>
+        <v>1</v>
+      </c>
+      <c r="AH34" s="10">
+        <f>EXP(AH27-AD27)</f>
+        <v>1</v>
+      </c>
+      <c r="AI34" s="10">
+        <f>EXP(AI27-AE27)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ34" s="10">
+        <f>EXP(AJ27-AF27)</f>
+        <v>1</v>
+      </c>
+      <c r="AK34" s="10">
+        <f>EXP(AK27-AG27)</f>
+        <v>1</v>
+      </c>
+      <c r="AL34" s="10">
+        <f>EXP(AL27-AH27)</f>
+        <v>1</v>
+      </c>
+      <c r="AM34" s="10">
+        <f>EXP(AM27-AI27)</f>
+        <v>1</v>
+      </c>
+      <c r="AN34" s="10">
+        <f>EXP(AN27-AJ27)</f>
+        <v>1</v>
+      </c>
+      <c r="AO34" s="10">
+        <f>EXP(AO27-AK27)</f>
+        <v>1</v>
+      </c>
+      <c r="AP34" s="10">
+        <f>EXP(AP27-AL27)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ34" s="10">
+        <f>EXP(AQ27-AM27)</f>
+        <v>1</v>
+      </c>
+      <c r="AR34" s="10">
+        <f>EXP(AR27-AN27)</f>
+        <v>1</v>
+      </c>
+      <c r="AS34" s="10">
+        <f>EXP(AS27-AO27)</f>
+        <v>1</v>
+      </c>
+      <c r="AT34" s="10">
+        <f>EXP(AT27-AP27)</f>
+        <v>1</v>
+      </c>
+      <c r="AU34" s="10">
+        <f>EXP(AU27-AQ27)</f>
+        <v>1</v>
+      </c>
+      <c r="AV34" s="10">
+        <f>EXP(AV27-AR27)</f>
+        <v>1</v>
+      </c>
+      <c r="AW34" s="10">
+        <f>EXP(AW27-AS27)</f>
+        <v>1</v>
+      </c>
+      <c r="AX34" s="10">
+        <f>EXP(AX27-AT27)</f>
+        <v>1</v>
+      </c>
+      <c r="AY34" s="10">
+        <f>EXP(AY27-AU27)</f>
+        <v>1</v>
+      </c>
+      <c r="AZ34" s="10">
+        <f>EXP(AZ27-AV27)</f>
+        <v>1</v>
+      </c>
+      <c r="BA34" s="10">
+        <f>EXP(BA27-AW27)</f>
+        <v>1</v>
+      </c>
+      <c r="BB34" s="10">
+        <f>EXP(BB27-AX27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:67" x14ac:dyDescent="0.3">
+      <c r="J35" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" s="10">
+        <f>EXP(K28-G28)</f>
+        <v>1</v>
+      </c>
+      <c r="L35" s="10">
+        <f>EXP(L28-H28)</f>
+        <v>1</v>
+      </c>
+      <c r="M35" s="10">
+        <f>EXP(M28-I28)</f>
+        <v>1</v>
+      </c>
+      <c r="N35" s="10">
+        <f>EXP(N28-J28)</f>
+        <v>1</v>
+      </c>
+      <c r="O35" s="10">
+        <f>EXP(O28-K28)</f>
+        <v>1</v>
+      </c>
+      <c r="P35" s="10">
+        <f>EXP(P28-L28)</f>
+        <v>1</v>
+      </c>
+      <c r="Q35" s="10">
+        <f>EXP(Q28-M28)</f>
+        <v>1</v>
+      </c>
+      <c r="R35" s="10">
+        <f>EXP(R28-N28)</f>
+        <v>1.2840254166877414</v>
+      </c>
+      <c r="S35" s="10">
+        <f>EXP(S28-O28)</f>
+        <v>1.6487212707001282</v>
+      </c>
+      <c r="T35" s="10">
+        <f>EXP(T28-P28)</f>
+        <v>2.1170000166126748</v>
+      </c>
+      <c r="U35" s="10">
+        <f>EXP(U28-Q28)</f>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="V35" s="10">
+        <f>EXP(V28-R28)</f>
+        <v>2.1170000166126748</v>
+      </c>
+      <c r="W35" s="10">
+        <f>EXP(W28-S28)</f>
+        <v>1.6487212707001282</v>
+      </c>
+      <c r="X35" s="10">
+        <f>EXP(X28-T28)</f>
+        <v>1.2840254166877414</v>
+      </c>
+      <c r="Y35" s="10">
+        <f>EXP(Y28-U28)</f>
+        <v>1</v>
+      </c>
+      <c r="Z35" s="10">
+        <f>EXP(Z28-V28)</f>
+        <v>1</v>
+      </c>
+      <c r="AA35" s="10">
+        <f>EXP(AA28-W28)</f>
+        <v>1</v>
+      </c>
+      <c r="AB35" s="10">
+        <f>EXP(AB28-X28)</f>
+        <v>1</v>
+      </c>
+      <c r="AC35" s="10">
+        <f>EXP(AC28-Y28)</f>
+        <v>1</v>
+      </c>
+      <c r="AD35" s="10">
+        <f>EXP(AD28-Z28)</f>
+        <v>1</v>
+      </c>
+      <c r="AE35" s="10">
+        <f>EXP(AE28-AA28)</f>
+        <v>1</v>
+      </c>
+      <c r="AF35" s="10">
+        <f>EXP(AF28-AB28)</f>
+        <v>1</v>
+      </c>
+      <c r="AG35" s="10">
+        <f>EXP(AG28-AC28)</f>
+        <v>1</v>
+      </c>
+      <c r="AH35" s="10">
+        <f>EXP(AH28-AD28)</f>
+        <v>1</v>
+      </c>
+      <c r="AI35" s="10">
+        <f>EXP(AI28-AE28)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ35" s="10">
+        <f>EXP(AJ28-AF28)</f>
+        <v>1</v>
+      </c>
+      <c r="AK35" s="10">
+        <f>EXP(AK28-AG28)</f>
+        <v>1</v>
+      </c>
+      <c r="AL35" s="10">
+        <f>EXP(AL28-AH28)</f>
+        <v>1</v>
+      </c>
+      <c r="AM35" s="10">
+        <f>EXP(AM28-AI28)</f>
+        <v>1</v>
+      </c>
+      <c r="AN35" s="10">
+        <f>EXP(AN28-AJ28)</f>
+        <v>1</v>
+      </c>
+      <c r="AO35" s="10">
+        <f>EXP(AO28-AK28)</f>
+        <v>1</v>
+      </c>
+      <c r="AP35" s="10">
+        <f>EXP(AP28-AL28)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ35" s="10">
+        <f>EXP(AQ28-AM28)</f>
+        <v>1</v>
+      </c>
+      <c r="AR35" s="10">
+        <f>EXP(AR28-AN28)</f>
+        <v>1</v>
+      </c>
+      <c r="AS35" s="10">
+        <f>EXP(AS28-AO28)</f>
+        <v>1</v>
+      </c>
+      <c r="AT35" s="10">
+        <f>EXP(AT28-AP28)</f>
+        <v>1</v>
+      </c>
+      <c r="AU35" s="10">
+        <f>EXP(AU28-AQ28)</f>
+        <v>1</v>
+      </c>
+      <c r="AV35" s="10">
+        <f>EXP(AV28-AR28)</f>
+        <v>1</v>
+      </c>
+      <c r="AW35" s="10">
+        <f>EXP(AW28-AS28)</f>
+        <v>1</v>
+      </c>
+      <c r="AX35" s="10">
+        <f>EXP(AX28-AT28)</f>
+        <v>1</v>
+      </c>
+      <c r="AY35" s="10">
+        <f>EXP(AY28-AU28)</f>
+        <v>1</v>
+      </c>
+      <c r="AZ35" s="10">
+        <f>EXP(AZ28-AV28)</f>
+        <v>1</v>
+      </c>
+      <c r="BA35" s="10">
+        <f>EXP(BA28-AW28)</f>
+        <v>1</v>
+      </c>
+      <c r="BB35" s="10">
+        <f>EXP(BB28-AX28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:67" x14ac:dyDescent="0.3">
+      <c r="J36" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K36" s="10">
+        <f>(K29/G29)</f>
+        <v>0.98927294806381083</v>
+      </c>
+      <c r="L36" s="10">
+        <f t="shared" ref="L36" si="1">(L29/H29)</f>
+        <v>0.99076079459272326</v>
+      </c>
+      <c r="M36" s="10">
+        <f t="shared" ref="M36" si="2">(M29/I29)</f>
+        <v>1.0158852555833802</v>
+      </c>
+      <c r="N36" s="10">
+        <f t="shared" ref="N36" si="3">(N29/J29)</f>
+        <v>1.0195911591816367</v>
+      </c>
+      <c r="O36" s="10">
+        <f t="shared" ref="O36" si="4">(O29/K29)</f>
+        <v>1.0108186700905004</v>
+      </c>
+      <c r="P36" s="10">
+        <f t="shared" ref="P36" si="5">(P29/L29)</f>
+        <v>1.0028578662191834</v>
+      </c>
+      <c r="Q36" s="10">
+        <f t="shared" ref="Q36" si="6">(Q29/M29)</f>
+        <v>1.0231662333573415</v>
+      </c>
+      <c r="R36" s="10">
+        <f t="shared" ref="R36" si="7">(R29/N29)</f>
+        <v>1.0061355802594669</v>
+      </c>
+      <c r="S36" s="10">
+        <f t="shared" ref="S36" si="8">(S29/O29)</f>
+        <v>1.0095551281822213</v>
+      </c>
+      <c r="T36" s="10">
+        <f t="shared" ref="T36" si="9">(T29/P29)</f>
+        <v>1.037833677960539</v>
+      </c>
+      <c r="U36" s="10">
+        <f t="shared" ref="U36" si="10">(U29/Q29)</f>
+        <v>0.97651158798075799</v>
+      </c>
+      <c r="V36" s="10">
+        <f t="shared" ref="V36" si="11">(V29/R29)</f>
+        <v>0.97658149609386757</v>
+      </c>
+      <c r="W36" s="10">
+        <f t="shared" ref="W36" si="12">(W29/S29)</f>
+        <v>0.98542598968653849</v>
+      </c>
+      <c r="X36" s="10">
+        <f t="shared" ref="X36" si="13">(X29/T29)</f>
+        <v>1.0037545696832597</v>
+      </c>
+      <c r="Y36" s="10">
+        <f t="shared" ref="Y36" si="14">(Y29/U29)</f>
+        <v>1.0504663580821358</v>
+      </c>
+      <c r="Z36" s="10">
+        <f t="shared" ref="Z36" si="15">(Z29/V29)</f>
+        <v>1.0633541380982423</v>
+      </c>
+      <c r="AA36" s="10">
+        <f t="shared" ref="AA36" si="16">(AA29/W29)</f>
+        <v>1.0634281815274489</v>
+      </c>
+      <c r="AB36" s="10">
+        <f t="shared" ref="AB36" si="17">(AB29/X29)</f>
+        <v>1.0170596464316353</v>
+      </c>
+      <c r="AC36" s="10">
+        <f t="shared" ref="AC36" si="18">(AC29/Y29)</f>
+        <v>1.0215458543512672</v>
+      </c>
+      <c r="AD36" s="10">
+        <f t="shared" ref="AD36" si="19">(AD29/Z29)</f>
+        <v>0.9912385224811292</v>
+      </c>
+      <c r="AE36" s="10">
+        <f t="shared" ref="AE36" si="20">(AE29/AA29)</f>
+        <v>0.9868049305494927</v>
+      </c>
+      <c r="AF36" s="10">
+        <f t="shared" ref="AF36" si="21">(AF29/AB29)</f>
+        <v>0.99997293995861491</v>
+      </c>
+      <c r="AG36" s="10">
+        <f t="shared" ref="AG36" si="22">(AG29/AC29)</f>
+        <v>0.97512083195064214</v>
+      </c>
+      <c r="AH36" s="10">
+        <f t="shared" ref="AH36" si="23">(AH29/AD29)</f>
+        <v>1.0126665564943758</v>
+      </c>
+      <c r="AI36" s="10">
+        <f t="shared" ref="AI36" si="24">(AI29/AE29)</f>
+        <v>1.0105522135814189</v>
+      </c>
+      <c r="AJ36" s="10">
+        <f t="shared" ref="AJ36" si="25">(AJ29/AF29)</f>
+        <v>0.9286652643770601</v>
+      </c>
+      <c r="AK36" s="10">
+        <f t="shared" ref="AK36" si="26">(AK29/AG29)</f>
+        <v>0.93429060338161229</v>
+      </c>
+      <c r="AL36" s="10">
+        <f t="shared" ref="AL36" si="27">(AL29/AH29)</f>
+        <v>0.91485899518932068</v>
+      </c>
+      <c r="AM36" s="10">
+        <f t="shared" ref="AM36" si="28">(AM29/AI29)</f>
+        <v>0.89113832927969772</v>
+      </c>
+      <c r="AN36" s="10">
+        <f t="shared" ref="AN36" si="29">(AN29/AJ29)</f>
+        <v>0.84007900197980068</v>
+      </c>
+      <c r="AO36" s="10">
+        <f t="shared" ref="AO36" si="30">(AO29/AK29)</f>
+        <v>0.98231801591735024</v>
+      </c>
+      <c r="AP36" s="10">
+        <f t="shared" ref="AP36" si="31">(AP29/AL29)</f>
+        <v>0.9863521598752949</v>
+      </c>
+      <c r="AQ36" s="10">
+        <f t="shared" ref="AQ36" si="32">(AQ29/AM29)</f>
+        <v>0.94729887059314688</v>
+      </c>
+      <c r="AR36" s="10">
+        <f t="shared" ref="AR36" si="33">(AR29/AN29)</f>
+        <v>1.2607689151799513</v>
+      </c>
+      <c r="AS36" s="10">
+        <f t="shared" ref="AS36" si="34">(AS29/AO29)</f>
+        <v>1.0572107803982338</v>
+      </c>
+      <c r="AT36" s="10">
+        <f t="shared" ref="AT36" si="35">(AT29/AP29)</f>
+        <v>1.0986522264414422</v>
+      </c>
+      <c r="AU36" s="10">
+        <f t="shared" ref="AU36" si="36">(AU29/AQ29)</f>
+        <v>1.1741982339434403</v>
+      </c>
+      <c r="AV36" s="10">
+        <f t="shared" ref="AV36" si="37">(AV29/AR29)</f>
+        <v>1.0243471530406525</v>
+      </c>
+      <c r="AW36" s="10">
+        <f t="shared" ref="AW36" si="38">(AW29/AS29)</f>
+        <v>1.0697086755441454</v>
+      </c>
+      <c r="AX36" s="10">
+        <f t="shared" ref="AX36" si="39">(AX29/AT29)</f>
+        <v>1.0314243240117227</v>
+      </c>
+      <c r="AY36" s="10">
+        <f t="shared" ref="AY36" si="40">(AY29/AU29)</f>
+        <v>1.0311630378317829</v>
+      </c>
+      <c r="AZ36" s="10">
+        <f t="shared" ref="AZ36" si="41">(AZ29/AV29)</f>
+        <v>1.0520845559325067</v>
+      </c>
+      <c r="BA36" s="10">
+        <f t="shared" ref="BA36" si="42">(BA29/AW29)</f>
+        <v>1.0706508708985307</v>
+      </c>
+      <c r="BB36" s="10">
+        <f t="shared" ref="BB36" si="43">(BB29/AX29)</f>
+        <v>0.98334633618663725</v>
+      </c>
+    </row>
+    <row r="37" spans="2:67" x14ac:dyDescent="0.3">
+      <c r="J37" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K37" s="10">
+        <f t="shared" ref="K37" si="44">(K30/G30)</f>
+        <v>1.0751285092492857</v>
+      </c>
+      <c r="L37" s="10">
+        <f t="shared" ref="L37" si="45">(L30/H30)</f>
+        <v>0.99988896480277778</v>
+      </c>
+      <c r="M37" s="10">
+        <f t="shared" ref="M37" si="46">(M30/I30)</f>
+        <v>1.0042974931098996</v>
+      </c>
+      <c r="N37" s="10">
+        <f t="shared" ref="N37" si="47">(N30/J30)</f>
+        <v>1.0263674994192997</v>
+      </c>
+      <c r="O37" s="10">
+        <f t="shared" ref="O37" si="48">(O30/K30)</f>
+        <v>1.0543785566305606</v>
+      </c>
+      <c r="P37" s="10">
+        <f t="shared" ref="P37" si="49">(P30/L30)</f>
+        <v>1.0464385133711949</v>
+      </c>
+      <c r="Q37" s="10">
+        <f t="shared" ref="Q37" si="50">(Q30/M30)</f>
+        <v>1.1108166788203855</v>
+      </c>
+      <c r="R37" s="10">
+        <f t="shared" ref="R37" si="51">(R30/N30)</f>
+        <v>1.0753214390598806</v>
+      </c>
+      <c r="S37" s="10">
+        <f t="shared" ref="S37" si="52">(S30/O30)</f>
+        <v>1.024534609485134</v>
+      </c>
+      <c r="T37" s="10">
+        <f t="shared" ref="T37" si="53">(T30/P30)</f>
+        <v>1.0626363243598227</v>
+      </c>
+      <c r="U37" s="10">
+        <f t="shared" ref="U37" si="54">(U30/Q30)</f>
+        <v>0.99724679431484642</v>
+      </c>
+      <c r="V37" s="10">
+        <f t="shared" ref="V37" si="55">(V30/R30)</f>
+        <v>0.99593316420274436</v>
+      </c>
+      <c r="W37" s="10">
+        <f t="shared" ref="W37" si="56">(W30/S30)</f>
+        <v>1.0210769361276515</v>
+      </c>
+      <c r="X37" s="10">
+        <f t="shared" ref="X37" si="57">(X30/T30)</f>
+        <v>1.0042855704237894</v>
+      </c>
+      <c r="Y37" s="10">
+        <f t="shared" ref="Y37" si="58">(Y30/U30)</f>
+        <v>1.0321787478549771</v>
+      </c>
+      <c r="Z37" s="10">
+        <f t="shared" ref="Z37" si="59">(Z30/V30)</f>
+        <v>1.0648518680367864</v>
+      </c>
+      <c r="AA37" s="10">
+        <f t="shared" ref="AA37" si="60">(AA30/W30)</f>
+        <v>1.0624733862190625</v>
+      </c>
+      <c r="AB37" s="10">
+        <f t="shared" ref="AB37" si="61">(AB30/X30)</f>
+        <v>1.0643079404231068</v>
+      </c>
+      <c r="AC37" s="10">
+        <f t="shared" ref="AC37" si="62">(AC30/Y30)</f>
+        <v>1.0558764809122887</v>
+      </c>
+      <c r="AD37" s="10">
+        <f t="shared" ref="AD37" si="63">(AD30/Z30)</f>
+        <v>1.0681678435528732</v>
+      </c>
+      <c r="AE37" s="10">
+        <f t="shared" ref="AE37" si="64">(AE30/AA30)</f>
+        <v>1.0462095323248883</v>
+      </c>
+      <c r="AF37" s="10">
+        <f t="shared" ref="AF37" si="65">(AF30/AB30)</f>
+        <v>1.0482329025953716</v>
+      </c>
+      <c r="AG37" s="10">
+        <f t="shared" ref="AG37" si="66">(AG30/AC30)</f>
+        <v>1.040245568769832</v>
+      </c>
+      <c r="AH37" s="10">
+        <f t="shared" ref="AH37" si="67">(AH30/AD30)</f>
+        <v>1.0189592040974371</v>
+      </c>
+      <c r="AI37" s="10">
+        <f t="shared" ref="AI37" si="68">(AI30/AE30)</f>
+        <v>1.00269906746167</v>
+      </c>
+      <c r="AJ37" s="10">
+        <f t="shared" ref="AJ37" si="69">(AJ30/AF30)</f>
+        <v>1.0090962298128385</v>
+      </c>
+      <c r="AK37" s="10">
+        <f t="shared" ref="AK37" si="70">(AK30/AG30)</f>
+        <v>0.99146215298535501</v>
+      </c>
+      <c r="AL37" s="10">
+        <f t="shared" ref="AL37" si="71">(AL30/AH30)</f>
+        <v>1.0165940359427574</v>
+      </c>
+      <c r="AM37" s="10">
+        <f t="shared" ref="AM37" si="72">(AM30/AI30)</f>
+        <v>0.96904003317694032</v>
+      </c>
+      <c r="AN37" s="10">
+        <f t="shared" ref="AN37" si="73">(AN30/AJ30)</f>
+        <v>0.69401402698374104</v>
+      </c>
+      <c r="AO37" s="10">
+        <f t="shared" ref="AO37" si="74">(AO30/AK30)</f>
+        <v>0.85702881166432499</v>
+      </c>
+      <c r="AP37" s="10">
+        <f t="shared" ref="AP37" si="75">(AP30/AL30)</f>
+        <v>0.78568116465731741</v>
+      </c>
+      <c r="AQ37" s="10">
+        <f t="shared" ref="AQ37" si="76">(AQ30/AM30)</f>
+        <v>0.74956571982661402</v>
+      </c>
+      <c r="AR37" s="10">
+        <f t="shared" ref="AR37" si="77">(AR30/AN30)</f>
+        <v>1.2798005516502784</v>
+      </c>
+      <c r="AS37" s="10">
+        <f t="shared" ref="AS37" si="78">(AS30/AO30)</f>
+        <v>1.0960647813587419</v>
+      </c>
+      <c r="AT37" s="10">
+        <f t="shared" ref="AT37" si="79">(AT30/AP30)</f>
+        <v>1.2719737593175151</v>
+      </c>
+      <c r="AU37" s="10">
+        <f t="shared" ref="AU37" si="80">(AU30/AQ30)</f>
+        <v>1.2885011373299213</v>
+      </c>
+      <c r="AV37" s="10">
+        <f t="shared" ref="AV37" si="81">(AV30/AR30)</f>
+        <v>1.1592923964455706</v>
+      </c>
+      <c r="AW37" s="10">
+        <f t="shared" ref="AW37" si="82">(AW30/AS30)</f>
+        <v>1.1634006772449141</v>
+      </c>
+      <c r="AX37" s="10">
+        <f t="shared" ref="AX37" si="83">(AX30/AT30)</f>
+        <v>1.0755044152407365</v>
+      </c>
+      <c r="AY37" s="10">
+        <f t="shared" ref="AY37" si="84">(AY30/AU30)</f>
+        <v>1.236796436185972</v>
+      </c>
+      <c r="AZ37" s="10">
+        <f t="shared" ref="AZ37" si="85">(AZ30/AV30)</f>
+        <v>1.1672996185911448</v>
+      </c>
+      <c r="BA37" s="10">
+        <f t="shared" ref="BA37" si="86">(BA30/AW30)</f>
+        <v>1.162151633648705</v>
+      </c>
+      <c r="BB37" s="10">
+        <f t="shared" ref="BB37" si="87">(BB30/AX30)</f>
+        <v>0.95315065005230692</v>
       </c>
     </row>
     <row r="40" spans="2:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4328,6 +5429,1092 @@
       <c r="BN40" s="1"/>
       <c r="BO40" s="1"/>
     </row>
+    <row r="42" spans="2:67" x14ac:dyDescent="0.3">
+      <c r="J42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K42" s="10">
+        <f>K14/G14</f>
+        <v>1.0727648191764818</v>
+      </c>
+      <c r="L42" s="10">
+        <f t="shared" ref="L42:BB47" si="88">L14/H14</f>
+        <v>1.1397977185581574</v>
+      </c>
+      <c r="M42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1520009582739563</v>
+      </c>
+      <c r="N42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1715230201452058</v>
+      </c>
+      <c r="O42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1756113959562653</v>
+      </c>
+      <c r="P42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1608373866356165</v>
+      </c>
+      <c r="Q42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.146021242663229</v>
+      </c>
+      <c r="R42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1330965856122193</v>
+      </c>
+      <c r="S42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1529562205401047</v>
+      </c>
+      <c r="T42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1562056493237611</v>
+      </c>
+      <c r="U42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1725467848212685</v>
+      </c>
+      <c r="V42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1343978983990528</v>
+      </c>
+      <c r="W42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1259750425223303</v>
+      </c>
+      <c r="X42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1382282728431885</v>
+      </c>
+      <c r="Y42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1181068310173008</v>
+      </c>
+      <c r="Z42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1184406293169278</v>
+      </c>
+      <c r="AA42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1520606571307064</v>
+      </c>
+      <c r="AB42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1438419835213089</v>
+      </c>
+      <c r="AC42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1218715197138667</v>
+      </c>
+      <c r="AD42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0987024334390365</v>
+      </c>
+      <c r="AE42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0757294137688815</v>
+      </c>
+      <c r="AF42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0710010950881486</v>
+      </c>
+      <c r="AG42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0767377495863317</v>
+      </c>
+      <c r="AH42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0989070968612422</v>
+      </c>
+      <c r="AI42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1000817190915169</v>
+      </c>
+      <c r="AJ42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0724409172857547</v>
+      </c>
+      <c r="AK42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0714108816246122</v>
+      </c>
+      <c r="AL42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0658284162481058</v>
+      </c>
+      <c r="AM42" s="10">
+        <f t="shared" si="88"/>
+        <v>0.90766919774459198</v>
+      </c>
+      <c r="AN42" s="10">
+        <f t="shared" si="88"/>
+        <v>0.57842182125473574</v>
+      </c>
+      <c r="AO42" s="10">
+        <f t="shared" si="88"/>
+        <v>0.90652149126932768</v>
+      </c>
+      <c r="AP42" s="10">
+        <f t="shared" si="88"/>
+        <v>0.7770265021689452</v>
+      </c>
+      <c r="AQ42" s="10">
+        <f t="shared" si="88"/>
+        <v>0.77442477940764165</v>
+      </c>
+      <c r="AR42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.6520064257546547</v>
+      </c>
+      <c r="AS42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1305041958749138</v>
+      </c>
+      <c r="AT42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.3173459951556687</v>
+      </c>
+      <c r="AU42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.4742951728457361</v>
+      </c>
+      <c r="AV42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1218623764035414</v>
+      </c>
+      <c r="AW42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.085090964839849</v>
+      </c>
+      <c r="AX42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.042585409674827</v>
+      </c>
+      <c r="AY42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1247803287230975</v>
+      </c>
+      <c r="AZ42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1240677340621057</v>
+      </c>
+      <c r="BA42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0961496537970725</v>
+      </c>
+      <c r="BB42" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0972641992115637</v>
+      </c>
+    </row>
+    <row r="43" spans="2:67" x14ac:dyDescent="0.3">
+      <c r="J43" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K43" s="10">
+        <f t="shared" ref="K43:K47" si="89">K15/G15</f>
+        <v>1.0059982209821259</v>
+      </c>
+      <c r="L43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0930944111941234</v>
+      </c>
+      <c r="M43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1385747263239276</v>
+      </c>
+      <c r="N43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1653772093469632</v>
+      </c>
+      <c r="O43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1416570778948494</v>
+      </c>
+      <c r="P43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1372794830411861</v>
+      </c>
+      <c r="Q43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1535795768476571</v>
+      </c>
+      <c r="R43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1736203684505295</v>
+      </c>
+      <c r="S43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2064009252206194</v>
+      </c>
+      <c r="T43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2635919640823563</v>
+      </c>
+      <c r="U43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.3047644447134259</v>
+      </c>
+      <c r="V43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1672085670462398</v>
+      </c>
+      <c r="W43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2080763262047616</v>
+      </c>
+      <c r="X43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1830431503229424</v>
+      </c>
+      <c r="Y43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1542590892145381</v>
+      </c>
+      <c r="Z43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1697365659349173</v>
+      </c>
+      <c r="AA43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1476704821034602</v>
+      </c>
+      <c r="AB43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1493968119397238</v>
+      </c>
+      <c r="AC43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.126995281949462</v>
+      </c>
+      <c r="AD43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1502503579233125</v>
+      </c>
+      <c r="AE43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1472258242597464</v>
+      </c>
+      <c r="AF43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1251808903396063</v>
+      </c>
+      <c r="AG43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1073777497287174</v>
+      </c>
+      <c r="AH43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1421251916604807</v>
+      </c>
+      <c r="AI43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1129946576594443</v>
+      </c>
+      <c r="AJ43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.108512755084734</v>
+      </c>
+      <c r="AK43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0954878655501088</v>
+      </c>
+      <c r="AL43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1078420257681048</v>
+      </c>
+      <c r="AM43" s="10">
+        <f t="shared" si="88"/>
+        <v>0.95378545950449811</v>
+      </c>
+      <c r="AN43" s="10">
+        <f t="shared" si="88"/>
+        <v>0.58283405447035674</v>
+      </c>
+      <c r="AO43" s="10">
+        <f t="shared" si="88"/>
+        <v>0.92935255064925504</v>
+      </c>
+      <c r="AP43" s="10">
+        <f t="shared" si="88"/>
+        <v>0.77330498402038927</v>
+      </c>
+      <c r="AQ43" s="10">
+        <f t="shared" si="88"/>
+        <v>0.76898767592314143</v>
+      </c>
+      <c r="AR43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.6897807936581952</v>
+      </c>
+      <c r="AS43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1646171228276914</v>
+      </c>
+      <c r="AT43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.425581036178251</v>
+      </c>
+      <c r="AU43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.5128887031993179</v>
+      </c>
+      <c r="AV43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1697075833145363</v>
+      </c>
+      <c r="AW43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1353564372617333</v>
+      </c>
+      <c r="AX43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0537772124786398</v>
+      </c>
+      <c r="AY43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1901849431397395</v>
+      </c>
+      <c r="AZ43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1743981598057487</v>
+      </c>
+      <c r="BA43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0626267636240765</v>
+      </c>
+      <c r="BB43" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1335535182780978</v>
+      </c>
+    </row>
+    <row r="44" spans="2:67" x14ac:dyDescent="0.3">
+      <c r="J44" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K44" s="10">
+        <f t="shared" si="89"/>
+        <v>0.92196844960627855</v>
+      </c>
+      <c r="L44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0101090687241756</v>
+      </c>
+      <c r="M44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0798808501840054</v>
+      </c>
+      <c r="N44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1206502259802102</v>
+      </c>
+      <c r="O44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1810419323832233</v>
+      </c>
+      <c r="P44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1544012366797174</v>
+      </c>
+      <c r="Q44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0854738557184043</v>
+      </c>
+      <c r="R44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1150810845821157</v>
+      </c>
+      <c r="S44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1154671223751358</v>
+      </c>
+      <c r="T44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1355675317714253</v>
+      </c>
+      <c r="U44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1420977361825166</v>
+      </c>
+      <c r="V44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.095510053151586</v>
+      </c>
+      <c r="W44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1692525982311768</v>
+      </c>
+      <c r="X44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1776790971501201</v>
+      </c>
+      <c r="Y44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1536963124695281</v>
+      </c>
+      <c r="Z44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1368770069449627</v>
+      </c>
+      <c r="AA44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0840334568523025</v>
+      </c>
+      <c r="AB44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0908460424136062</v>
+      </c>
+      <c r="AC44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0847326496047307</v>
+      </c>
+      <c r="AD44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.121277568458058</v>
+      </c>
+      <c r="AE44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1267624245787098</v>
+      </c>
+      <c r="AF44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1029448831338853</v>
+      </c>
+      <c r="AG44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0962249164107216</v>
+      </c>
+      <c r="AH44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1424736851971617</v>
+      </c>
+      <c r="AI44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1519727668102868</v>
+      </c>
+      <c r="AJ44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1252716605015436</v>
+      </c>
+      <c r="AK44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1307576631339038</v>
+      </c>
+      <c r="AL44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1180158237746318</v>
+      </c>
+      <c r="AM44" s="10">
+        <f t="shared" si="88"/>
+        <v>0.96120898520445675</v>
+      </c>
+      <c r="AN44" s="10">
+        <f t="shared" si="88"/>
+        <v>0.62147269978120223</v>
+      </c>
+      <c r="AO44" s="10">
+        <f t="shared" si="88"/>
+        <v>0.94631164322222838</v>
+      </c>
+      <c r="AP44" s="10">
+        <f t="shared" si="88"/>
+        <v>0.79692696896148763</v>
+      </c>
+      <c r="AQ44" s="10">
+        <f t="shared" si="88"/>
+        <v>0.79202118671308874</v>
+      </c>
+      <c r="AR44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.6711527456233901</v>
+      </c>
+      <c r="AS44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1710766263370158</v>
+      </c>
+      <c r="AT44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.4093640114870425</v>
+      </c>
+      <c r="AU44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.4879925000385081</v>
+      </c>
+      <c r="AV44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.140079929487716</v>
+      </c>
+      <c r="AW44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1231135563236843</v>
+      </c>
+      <c r="AX44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.059889951713507</v>
+      </c>
+      <c r="AY44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1447149314837095</v>
+      </c>
+      <c r="AZ44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1242504661253783</v>
+      </c>
+      <c r="BA44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0138858173548213</v>
+      </c>
+      <c r="BB44" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0674936844826475</v>
+      </c>
+    </row>
+    <row r="45" spans="2:67" x14ac:dyDescent="0.3">
+      <c r="J45" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K45" s="10">
+        <f t="shared" si="89"/>
+        <v>1.1790048297684292</v>
+      </c>
+      <c r="L45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2202021410050075</v>
+      </c>
+      <c r="M45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1654658148013204</v>
+      </c>
+      <c r="N45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2065492410688174</v>
+      </c>
+      <c r="O45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2434745440899682</v>
+      </c>
+      <c r="P45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2943471523340422</v>
+      </c>
+      <c r="Q45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2620058424766711</v>
+      </c>
+      <c r="R45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2007019138572541</v>
+      </c>
+      <c r="S45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1504205732288872</v>
+      </c>
+      <c r="T45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1308447436207096</v>
+      </c>
+      <c r="U45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1138632313879766</v>
+      </c>
+      <c r="V45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1531111326241512</v>
+      </c>
+      <c r="W45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1647861874014138</v>
+      </c>
+      <c r="X45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2105852971540294</v>
+      </c>
+      <c r="Y45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1638312418862879</v>
+      </c>
+      <c r="Z45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1482846772600566</v>
+      </c>
+      <c r="AA45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1834358031169765</v>
+      </c>
+      <c r="AB45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1226826600700421</v>
+      </c>
+      <c r="AC45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1488855511796054</v>
+      </c>
+      <c r="AD45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1008432234794168</v>
+      </c>
+      <c r="AE45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0657358550790994</v>
+      </c>
+      <c r="AF45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1015139479101173</v>
+      </c>
+      <c r="AG45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0615421063880592</v>
+      </c>
+      <c r="AH45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.110803931785372</v>
+      </c>
+      <c r="AI45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1275879683821664</v>
+      </c>
+      <c r="AJ45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0479767152758392</v>
+      </c>
+      <c r="AK45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.101084640762571</v>
+      </c>
+      <c r="AL45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0879174138774446</v>
+      </c>
+      <c r="AM45" s="10">
+        <f t="shared" si="88"/>
+        <v>0.99238864399333959</v>
+      </c>
+      <c r="AN45" s="10">
+        <f t="shared" si="88"/>
+        <v>0.81590254904676174</v>
+      </c>
+      <c r="AO45" s="10">
+        <f t="shared" si="88"/>
+        <v>0.95797892925262274</v>
+      </c>
+      <c r="AP45" s="10">
+        <f t="shared" si="88"/>
+        <v>0.92132959098544009</v>
+      </c>
+      <c r="AQ45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0022168616889089</v>
+      </c>
+      <c r="AR45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.3386613333768798</v>
+      </c>
+      <c r="AS45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.111283011615342</v>
+      </c>
+      <c r="AT45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1812332284732081</v>
+      </c>
+      <c r="AU45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1619639368380594</v>
+      </c>
+      <c r="AV45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0702764032237249</v>
+      </c>
+      <c r="AW45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0732570609340377</v>
+      </c>
+      <c r="AX45" s="10">
+        <f t="shared" si="88"/>
+        <v>0.97074301358998749</v>
+      </c>
+      <c r="AY45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0709855748418096</v>
+      </c>
+      <c r="AZ45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0730976759080224</v>
+      </c>
+      <c r="BA45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0298950547875421</v>
+      </c>
+      <c r="BB45" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1220592837373575</v>
+      </c>
+    </row>
+    <row r="46" spans="2:67" x14ac:dyDescent="0.3">
+      <c r="J46" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K46" s="10">
+        <f t="shared" si="89"/>
+        <v>0.99347416959906731</v>
+      </c>
+      <c r="L46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0842147941297187</v>
+      </c>
+      <c r="M46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0662625799538052</v>
+      </c>
+      <c r="N46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0937804512575158</v>
+      </c>
+      <c r="O46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1741608551855647</v>
+      </c>
+      <c r="P46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1770827313289833</v>
+      </c>
+      <c r="Q46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2341951436365808</v>
+      </c>
+      <c r="R46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2479324212937759</v>
+      </c>
+      <c r="S46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2504885969982653</v>
+      </c>
+      <c r="T46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2822470911358204</v>
+      </c>
+      <c r="U46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2738516911049309</v>
+      </c>
+      <c r="V46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2056699644542999</v>
+      </c>
+      <c r="W46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1571355116626916</v>
+      </c>
+      <c r="X46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1563545158080575</v>
+      </c>
+      <c r="Y46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.115028534612347</v>
+      </c>
+      <c r="Z46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1291494898916945</v>
+      </c>
+      <c r="AA46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.178720635414455</v>
+      </c>
+      <c r="AB46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1516388147537415</v>
+      </c>
+      <c r="AC46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1333571414720305</v>
+      </c>
+      <c r="AD46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1617353151680232</v>
+      </c>
+      <c r="AE46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.166403651067204</v>
+      </c>
+      <c r="AF46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.148138762391629</v>
+      </c>
+      <c r="AG46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1163602589405934</v>
+      </c>
+      <c r="AH46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1731577727210549</v>
+      </c>
+      <c r="AI46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1341308404245303</v>
+      </c>
+      <c r="AJ46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0973808352433976</v>
+      </c>
+      <c r="AK46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1465629732008598</v>
+      </c>
+      <c r="AL46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1244576054390572</v>
+      </c>
+      <c r="AM46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0554191485099624</v>
+      </c>
+      <c r="AN46" s="10">
+        <f t="shared" si="88"/>
+        <v>0.76954473394927214</v>
+      </c>
+      <c r="AO46" s="10">
+        <f t="shared" si="88"/>
+        <v>0.97163317371178914</v>
+      </c>
+      <c r="AP46" s="10">
+        <f t="shared" si="88"/>
+        <v>0.92502222892620645</v>
+      </c>
+      <c r="AQ46" s="10">
+        <f t="shared" si="88"/>
+        <v>0.9575921673074379</v>
+      </c>
+      <c r="AR46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.4227708321884631</v>
+      </c>
+      <c r="AS46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1135946050787082</v>
+      </c>
+      <c r="AT46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.22696856719712</v>
+      </c>
+      <c r="AU46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2083930324171448</v>
+      </c>
+      <c r="AV46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0889000291357425</v>
+      </c>
+      <c r="AW46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1069688918009883</v>
+      </c>
+      <c r="AX46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.032605536756283</v>
+      </c>
+      <c r="AY46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0874664384908421</v>
+      </c>
+      <c r="AZ46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.085857522312843</v>
+      </c>
+      <c r="BA46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0535049730328669</v>
+      </c>
+      <c r="BB46" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0855390815751704</v>
+      </c>
+    </row>
+    <row r="47" spans="2:67" x14ac:dyDescent="0.3">
+      <c r="J47" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K47" s="10">
+        <f t="shared" si="89"/>
+        <v>1.0504004342561277</v>
+      </c>
+      <c r="L47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0273769100169781</v>
+      </c>
+      <c r="M47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1065627522195316</v>
+      </c>
+      <c r="N47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1746170904027646</v>
+      </c>
+      <c r="O47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0303381083297158</v>
+      </c>
+      <c r="P47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1809801693864901</v>
+      </c>
+      <c r="Q47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0430788867868619</v>
+      </c>
+      <c r="R47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0686657593186106</v>
+      </c>
+      <c r="S47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.182660799550604</v>
+      </c>
+      <c r="T47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1744102149244593</v>
+      </c>
+      <c r="U47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2032864978257547</v>
+      </c>
+      <c r="V47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1624419703381128</v>
+      </c>
+      <c r="W47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1511972036829541</v>
+      </c>
+      <c r="X47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2005622370331757</v>
+      </c>
+      <c r="Y47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1513638179638979</v>
+      </c>
+      <c r="Z47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.118801908464393</v>
+      </c>
+      <c r="AA47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1197624904123356</v>
+      </c>
+      <c r="AB47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0815823344239923</v>
+      </c>
+      <c r="AC47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1579785807794829</v>
+      </c>
+      <c r="AD47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1984268633613953</v>
+      </c>
+      <c r="AE47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1374857985076918</v>
+      </c>
+      <c r="AF47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1608361530079716</v>
+      </c>
+      <c r="AG47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.110097116471662</v>
+      </c>
+      <c r="AH47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1694079814434075</v>
+      </c>
+      <c r="AI47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2171307481542468</v>
+      </c>
+      <c r="AJ47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.2088036953783068</v>
+      </c>
+      <c r="AK47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1679877300613497</v>
+      </c>
+      <c r="AL47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.1912769074721064</v>
+      </c>
+      <c r="AM47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0577118055826362</v>
+      </c>
+      <c r="AN47" s="10">
+        <f t="shared" si="88"/>
+        <v>0.75245218244237388</v>
+      </c>
+      <c r="AO47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0222079818470236</v>
+      </c>
+      <c r="AP47" s="10">
+        <f t="shared" si="88"/>
+        <v>0.921269228586025</v>
+      </c>
+      <c r="AQ47" s="10">
+        <f t="shared" si="88"/>
+        <v>0.96404684547675012</v>
+      </c>
+      <c r="AR47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.6403644560317201</v>
+      </c>
+      <c r="AS47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.288258568418889</v>
+      </c>
+      <c r="AT47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.3544362292051753</v>
+      </c>
+      <c r="AU47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.3138410675250947</v>
+      </c>
+      <c r="AV47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0165310464144102</v>
+      </c>
+      <c r="AW47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0199514973594779</v>
+      </c>
+      <c r="AX47" s="10">
+        <f t="shared" si="88"/>
+        <v>0.99851396944539228</v>
+      </c>
+      <c r="AY47" s="10">
+        <f t="shared" si="88"/>
+        <v>1.0956302924450996</v>
+      </c>
+      <c r="AZ47" s="10">
+        <f t="shared" ref="AZ47" si="90">AZ19/AV19</f>
+        <v>1.1066612377850167</v>
+      </c>
+      <c r="BA47" s="10">
+        <f t="shared" ref="BA47" si="91">BA19/AW19</f>
+        <v>1.031261976457706</v>
+      </c>
+      <c r="BB47" s="10">
+        <f t="shared" ref="BB47" si="92">BB19/AX19</f>
+        <v>0.9933864342174199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup paperSize="9" scale="57" orientation="portrait"/>

</xml_diff>

<commit_message>
added regression ranking page, moved backcast functionality in that page, added timestep on template ssheets on cells H50 for now
</commit_message>
<xml_diff>
--- a/data/reg_input/Development Test Data Regression Inputs.xlsx
+++ b/data/reg_input/Development Test Data Regression Inputs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fidias\Coding-related\Python\Traffic-Regression-Tool\data\reg_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC20670-9E83-4C1B-B64C-8B9F7256498F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86B4478-D26B-4279-8AD1-5ACDFA4FAFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30840" yWindow="-120" windowWidth="30030" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33880" yWindow="-6390" windowWidth="13650" windowHeight="7960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="76">
   <si>
     <t>Confidential</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>pct_val_or_dummy</t>
+  </si>
+  <si>
+    <t>Timestep</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
   </si>
 </sst>
 </file>
@@ -1264,10 +1270,10 @@
     <tabColor theme="6" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BO47"/>
+  <dimension ref="B2:BO50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4459,179 +4465,179 @@
         <v>67</v>
       </c>
       <c r="K33" s="10">
-        <f>EXP(K26-G26)</f>
+        <f t="shared" ref="K33:T35" si="1">EXP(K26-G26)</f>
         <v>16.444646771097062</v>
       </c>
       <c r="L33" s="10">
-        <f>EXP(L26-H26)</f>
+        <f t="shared" si="1"/>
         <v>4.9530324243951043</v>
       </c>
       <c r="M33" s="10">
-        <f>EXP(M26-I26)</f>
+        <f t="shared" si="1"/>
         <v>0.74081822068171732</v>
       </c>
       <c r="N33" s="10">
-        <f>EXP(N26-J26)</f>
+        <f t="shared" si="1"/>
         <v>0.18268352405273477</v>
       </c>
       <c r="O33" s="10">
-        <f>EXP(O26-K26)</f>
+        <f t="shared" si="1"/>
         <v>6.7205512739749812E-2</v>
       </c>
       <c r="P33" s="10">
-        <f>EXP(P26-L26)</f>
+        <f t="shared" si="1"/>
         <v>6.0810062625218028E-2</v>
       </c>
       <c r="Q33" s="10">
-        <f>EXP(Q26-M26)</f>
+        <f t="shared" si="1"/>
         <v>6.7205512739749687E-2</v>
       </c>
       <c r="R33" s="10">
-        <f>EXP(R26-N26)</f>
+        <f t="shared" si="1"/>
         <v>0.12245642825298195</v>
       </c>
       <c r="S33" s="10">
-        <f>EXP(S26-O26)</f>
+        <f t="shared" si="1"/>
         <v>0.22313016014842982</v>
       </c>
       <c r="T33" s="10">
-        <f>EXP(T26-P26)</f>
+        <f t="shared" si="1"/>
         <v>0.11080315836233397</v>
       </c>
       <c r="U33" s="10">
-        <f>EXP(U26-Q26)</f>
+        <f t="shared" ref="U33:AD35" si="2">EXP(U26-Q26)</f>
         <v>0.27253179303401337</v>
       </c>
       <c r="V33" s="10">
-        <f>EXP(V26-R26)</f>
+        <f t="shared" si="2"/>
         <v>0.27253179303401193</v>
       </c>
       <c r="W33" s="10">
-        <f>EXP(W26-S26)</f>
+        <f t="shared" si="2"/>
         <v>0.22313016014842982</v>
       </c>
       <c r="X33" s="10">
-        <f>EXP(X26-T26)</f>
+        <f t="shared" si="2"/>
         <v>0.30119421191220175</v>
       </c>
       <c r="Y33" s="10">
-        <f>EXP(Y26-U26)</f>
+        <f t="shared" si="2"/>
         <v>0.22313016014842982</v>
       </c>
       <c r="Z33" s="10">
-        <f>EXP(Z26-V26)</f>
+        <f t="shared" si="2"/>
         <v>0.14956861922263526</v>
       </c>
       <c r="AA33" s="10">
-        <f>EXP(AA26-W26)</f>
+        <f t="shared" si="2"/>
         <v>9.071795328941247E-2</v>
       </c>
       <c r="AB33" s="10">
-        <f>EXP(AB26-X26)</f>
+        <f t="shared" si="2"/>
         <v>0.1353352832366127</v>
       </c>
       <c r="AC33" s="10">
-        <f>EXP(AC26-Y26)</f>
+        <f t="shared" si="2"/>
         <v>0.11080315836233376</v>
       </c>
       <c r="AD33" s="10">
-        <f>EXP(AD26-Z26)</f>
+        <f t="shared" si="2"/>
         <v>8.20849986238988E-2</v>
       </c>
       <c r="AE33" s="10">
-        <f>EXP(AE26-AA26)</f>
+        <f t="shared" ref="AE33:AN35" si="3">EXP(AE26-AA26)</f>
         <v>0.10025884372280366</v>
       </c>
       <c r="AF33" s="10">
-        <f>EXP(AF26-AB26)</f>
+        <f t="shared" si="3"/>
         <v>0.10025884372280384</v>
       </c>
       <c r="AG33" s="10">
-        <f>EXP(AG26-AC26)</f>
+        <f t="shared" si="3"/>
         <v>0.16529888822158673</v>
       </c>
       <c r="AH33" s="10">
-        <f>EXP(AH26-AD26)</f>
+        <f t="shared" si="3"/>
         <v>0.22313016014842982</v>
       </c>
       <c r="AI33" s="10">
-        <f>EXP(AI26-AE26)</f>
+        <f t="shared" si="3"/>
         <v>0.3011942119122023</v>
       </c>
       <c r="AJ33" s="10">
-        <f>EXP(AJ26-AF26)</f>
+        <f t="shared" si="3"/>
         <v>0.60653065971263342</v>
       </c>
       <c r="AK33" s="10">
-        <f>EXP(AK26-AG26)</f>
+        <f t="shared" si="3"/>
         <v>0.54881163609402617</v>
       </c>
       <c r="AL33" s="10">
-        <f>EXP(AL26-AH26)</f>
+        <f t="shared" si="3"/>
         <v>1.1051709180756473</v>
       </c>
       <c r="AM33" s="10">
-        <f>EXP(AM26-AI26)</f>
+        <f t="shared" si="3"/>
         <v>0.90483741803595985</v>
       </c>
       <c r="AN33" s="10">
-        <f>EXP(AN26-AJ26)</f>
+        <f t="shared" si="3"/>
         <v>0.49658530379140942</v>
       </c>
       <c r="AO33" s="10">
-        <f>EXP(AO26-AK26)</f>
+        <f t="shared" ref="AO33:AX35" si="4">EXP(AO26-AK26)</f>
         <v>5.4739473917272008</v>
       </c>
       <c r="AP33" s="10">
-        <f>EXP(AP26-AL26)</f>
+        <f t="shared" si="4"/>
         <v>1.4918246976412695</v>
       </c>
       <c r="AQ33" s="10">
-        <f>EXP(AQ26-AM26)</f>
+        <f t="shared" si="4"/>
         <v>1.3498588075760016</v>
       </c>
       <c r="AR33" s="10">
-        <f>EXP(AR26-AN26)</f>
+        <f t="shared" si="4"/>
         <v>2.7182818284590451</v>
       </c>
       <c r="AS33" s="10">
-        <f>EXP(AS26-AO26)</f>
+        <f t="shared" si="4"/>
         <v>0.14956861922263501</v>
       </c>
       <c r="AT33" s="10">
-        <f>EXP(AT26-AP26)</f>
+        <f t="shared" si="4"/>
         <v>0.36787944117144233</v>
       </c>
       <c r="AU33" s="10">
-        <f>EXP(AU26-AQ26)</f>
+        <f t="shared" si="4"/>
         <v>0.3011942119122023</v>
       </c>
       <c r="AV33" s="10">
-        <f>EXP(AV26-AR26)</f>
+        <f t="shared" si="4"/>
         <v>0.36787944117144233</v>
       </c>
       <c r="AW33" s="10">
-        <f>EXP(AW26-AS26)</f>
+        <f t="shared" si="4"/>
         <v>0.74081822068171799</v>
       </c>
       <c r="AX33" s="10">
-        <f>EXP(AX26-AT26)</f>
+        <f t="shared" si="4"/>
         <v>1.2214027581601701</v>
       </c>
       <c r="AY33" s="10">
-        <f>EXP(AY26-AU26)</f>
+        <f t="shared" ref="AY33:BB35" si="5">EXP(AY26-AU26)</f>
         <v>3.6692966676192467</v>
       </c>
       <c r="AZ33" s="10">
-        <f>EXP(AZ26-AV26)</f>
+        <f t="shared" si="5"/>
         <v>1.4918246976412695</v>
       </c>
       <c r="BA33" s="10">
-        <f>EXP(BA26-AW26)</f>
+        <f t="shared" si="5"/>
         <v>2.2255409284924692</v>
       </c>
       <c r="BB33" s="10">
-        <f>EXP(BB26-AX26)</f>
+        <f t="shared" si="5"/>
         <v>1.1051709180756482</v>
       </c>
     </row>
@@ -4640,179 +4646,179 @@
         <v>68</v>
       </c>
       <c r="K34" s="10">
-        <f>EXP(K27-G27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L34" s="10">
-        <f>EXP(L27-H27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M34" s="10">
-        <f>EXP(M27-I27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N34" s="10">
-        <f>EXP(N27-J27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O34" s="10">
-        <f>EXP(O27-K27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P34" s="10">
-        <f>EXP(P27-L27)</f>
+        <f t="shared" si="1"/>
         <v>2.7182818284590451</v>
       </c>
       <c r="Q34" s="10">
-        <f>EXP(Q27-M27)</f>
+        <f t="shared" si="1"/>
         <v>2.7182818284590451</v>
       </c>
       <c r="R34" s="10">
-        <f>EXP(R27-N27)</f>
+        <f t="shared" si="1"/>
         <v>2.7182818284590451</v>
       </c>
       <c r="S34" s="10">
-        <f>EXP(S27-O27)</f>
+        <f t="shared" si="1"/>
         <v>2.7182818284590451</v>
       </c>
       <c r="T34" s="10">
-        <f>EXP(T27-P27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="U34" s="10">
-        <f>EXP(U27-Q27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V34" s="10">
-        <f>EXP(V27-R27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="W34" s="10">
-        <f>EXP(W27-S27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="X34" s="10">
-        <f>EXP(X27-T27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Y34" s="10">
-        <f>EXP(Y27-U27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Z34" s="10">
-        <f>EXP(Z27-V27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AA34" s="10">
-        <f>EXP(AA27-W27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AB34" s="10">
-        <f>EXP(AB27-X27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AC34" s="10">
-        <f>EXP(AC27-Y27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD34" s="10">
-        <f>EXP(AD27-Z27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AE34" s="10">
-        <f>EXP(AE27-AA27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AF34" s="10">
-        <f>EXP(AF27-AB27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AG34" s="10">
-        <f>EXP(AG27-AC27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AH34" s="10">
-        <f>EXP(AH27-AD27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AI34" s="10">
-        <f>EXP(AI27-AE27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AJ34" s="10">
-        <f>EXP(AJ27-AF27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AK34" s="10">
-        <f>EXP(AK27-AG27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AL34" s="10">
-        <f>EXP(AL27-AH27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AM34" s="10">
-        <f>EXP(AM27-AI27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AN34" s="10">
-        <f>EXP(AN27-AJ27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AO34" s="10">
-        <f>EXP(AO27-AK27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AP34" s="10">
-        <f>EXP(AP27-AL27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AQ34" s="10">
-        <f>EXP(AQ27-AM27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AR34" s="10">
-        <f>EXP(AR27-AN27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AS34" s="10">
-        <f>EXP(AS27-AO27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AT34" s="10">
-        <f>EXP(AT27-AP27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AU34" s="10">
-        <f>EXP(AU27-AQ27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AV34" s="10">
-        <f>EXP(AV27-AR27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AW34" s="10">
-        <f>EXP(AW27-AS27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AX34" s="10">
-        <f>EXP(AX27-AT27)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AY34" s="10">
-        <f>EXP(AY27-AU27)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AZ34" s="10">
-        <f>EXP(AZ27-AV27)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="BA34" s="10">
-        <f>EXP(BA27-AW27)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="BB34" s="10">
-        <f>EXP(BB27-AX27)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -4821,179 +4827,179 @@
         <v>69</v>
       </c>
       <c r="K35" s="10">
-        <f>EXP(K28-G28)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L35" s="10">
-        <f>EXP(L28-H28)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M35" s="10">
-        <f>EXP(M28-I28)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N35" s="10">
-        <f>EXP(N28-J28)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O35" s="10">
-        <f>EXP(O28-K28)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P35" s="10">
-        <f>EXP(P28-L28)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q35" s="10">
-        <f>EXP(Q28-M28)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R35" s="10">
-        <f>EXP(R28-N28)</f>
+        <f t="shared" si="1"/>
         <v>1.2840254166877414</v>
       </c>
       <c r="S35" s="10">
-        <f>EXP(S28-O28)</f>
+        <f t="shared" si="1"/>
         <v>1.6487212707001282</v>
       </c>
       <c r="T35" s="10">
-        <f>EXP(T28-P28)</f>
+        <f t="shared" si="1"/>
         <v>2.1170000166126748</v>
       </c>
       <c r="U35" s="10">
-        <f>EXP(U28-Q28)</f>
+        <f t="shared" si="2"/>
         <v>2.7182818284590451</v>
       </c>
       <c r="V35" s="10">
-        <f>EXP(V28-R28)</f>
+        <f t="shared" si="2"/>
         <v>2.1170000166126748</v>
       </c>
       <c r="W35" s="10">
-        <f>EXP(W28-S28)</f>
+        <f t="shared" si="2"/>
         <v>1.6487212707001282</v>
       </c>
       <c r="X35" s="10">
-        <f>EXP(X28-T28)</f>
+        <f t="shared" si="2"/>
         <v>1.2840254166877414</v>
       </c>
       <c r="Y35" s="10">
-        <f>EXP(Y28-U28)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Z35" s="10">
-        <f>EXP(Z28-V28)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AA35" s="10">
-        <f>EXP(AA28-W28)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AB35" s="10">
-        <f>EXP(AB28-X28)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AC35" s="10">
-        <f>EXP(AC28-Y28)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD35" s="10">
-        <f>EXP(AD28-Z28)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AE35" s="10">
-        <f>EXP(AE28-AA28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AF35" s="10">
-        <f>EXP(AF28-AB28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AG35" s="10">
-        <f>EXP(AG28-AC28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AH35" s="10">
-        <f>EXP(AH28-AD28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AI35" s="10">
-        <f>EXP(AI28-AE28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AJ35" s="10">
-        <f>EXP(AJ28-AF28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AK35" s="10">
-        <f>EXP(AK28-AG28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AL35" s="10">
-        <f>EXP(AL28-AH28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AM35" s="10">
-        <f>EXP(AM28-AI28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AN35" s="10">
-        <f>EXP(AN28-AJ28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AO35" s="10">
-        <f>EXP(AO28-AK28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AP35" s="10">
-        <f>EXP(AP28-AL28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AQ35" s="10">
-        <f>EXP(AQ28-AM28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AR35" s="10">
-        <f>EXP(AR28-AN28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AS35" s="10">
-        <f>EXP(AS28-AO28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AT35" s="10">
-        <f>EXP(AT28-AP28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AU35" s="10">
-        <f>EXP(AU28-AQ28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AV35" s="10">
-        <f>EXP(AV28-AR28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AW35" s="10">
-        <f>EXP(AW28-AS28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AX35" s="10">
-        <f>EXP(AX28-AT28)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AY35" s="10">
-        <f>EXP(AY28-AU28)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AZ35" s="10">
-        <f>EXP(AZ28-AV28)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="BA35" s="10">
-        <f>EXP(BA28-AW28)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="BB35" s="10">
-        <f>EXP(BB28-AX28)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -5006,175 +5012,175 @@
         <v>0.98927294806381083</v>
       </c>
       <c r="L36" s="10">
-        <f t="shared" ref="L36" si="1">(L29/H29)</f>
+        <f t="shared" ref="L36" si="6">(L29/H29)</f>
         <v>0.99076079459272326</v>
       </c>
       <c r="M36" s="10">
-        <f t="shared" ref="M36" si="2">(M29/I29)</f>
+        <f t="shared" ref="M36" si="7">(M29/I29)</f>
         <v>1.0158852555833802</v>
       </c>
       <c r="N36" s="10">
-        <f t="shared" ref="N36" si="3">(N29/J29)</f>
+        <f t="shared" ref="N36" si="8">(N29/J29)</f>
         <v>1.0195911591816367</v>
       </c>
       <c r="O36" s="10">
-        <f t="shared" ref="O36" si="4">(O29/K29)</f>
+        <f t="shared" ref="O36" si="9">(O29/K29)</f>
         <v>1.0108186700905004</v>
       </c>
       <c r="P36" s="10">
-        <f t="shared" ref="P36" si="5">(P29/L29)</f>
+        <f t="shared" ref="P36" si="10">(P29/L29)</f>
         <v>1.0028578662191834</v>
       </c>
       <c r="Q36" s="10">
-        <f t="shared" ref="Q36" si="6">(Q29/M29)</f>
+        <f t="shared" ref="Q36" si="11">(Q29/M29)</f>
         <v>1.0231662333573415</v>
       </c>
       <c r="R36" s="10">
-        <f t="shared" ref="R36" si="7">(R29/N29)</f>
+        <f t="shared" ref="R36" si="12">(R29/N29)</f>
         <v>1.0061355802594669</v>
       </c>
       <c r="S36" s="10">
-        <f t="shared" ref="S36" si="8">(S29/O29)</f>
+        <f t="shared" ref="S36" si="13">(S29/O29)</f>
         <v>1.0095551281822213</v>
       </c>
       <c r="T36" s="10">
-        <f t="shared" ref="T36" si="9">(T29/P29)</f>
+        <f t="shared" ref="T36" si="14">(T29/P29)</f>
         <v>1.037833677960539</v>
       </c>
       <c r="U36" s="10">
-        <f t="shared" ref="U36" si="10">(U29/Q29)</f>
+        <f t="shared" ref="U36" si="15">(U29/Q29)</f>
         <v>0.97651158798075799</v>
       </c>
       <c r="V36" s="10">
-        <f t="shared" ref="V36" si="11">(V29/R29)</f>
+        <f t="shared" ref="V36" si="16">(V29/R29)</f>
         <v>0.97658149609386757</v>
       </c>
       <c r="W36" s="10">
-        <f t="shared" ref="W36" si="12">(W29/S29)</f>
+        <f t="shared" ref="W36" si="17">(W29/S29)</f>
         <v>0.98542598968653849</v>
       </c>
       <c r="X36" s="10">
-        <f t="shared" ref="X36" si="13">(X29/T29)</f>
+        <f t="shared" ref="X36" si="18">(X29/T29)</f>
         <v>1.0037545696832597</v>
       </c>
       <c r="Y36" s="10">
-        <f t="shared" ref="Y36" si="14">(Y29/U29)</f>
+        <f t="shared" ref="Y36" si="19">(Y29/U29)</f>
         <v>1.0504663580821358</v>
       </c>
       <c r="Z36" s="10">
-        <f t="shared" ref="Z36" si="15">(Z29/V29)</f>
+        <f t="shared" ref="Z36" si="20">(Z29/V29)</f>
         <v>1.0633541380982423</v>
       </c>
       <c r="AA36" s="10">
-        <f t="shared" ref="AA36" si="16">(AA29/W29)</f>
+        <f t="shared" ref="AA36" si="21">(AA29/W29)</f>
         <v>1.0634281815274489</v>
       </c>
       <c r="AB36" s="10">
-        <f t="shared" ref="AB36" si="17">(AB29/X29)</f>
+        <f t="shared" ref="AB36" si="22">(AB29/X29)</f>
         <v>1.0170596464316353</v>
       </c>
       <c r="AC36" s="10">
-        <f t="shared" ref="AC36" si="18">(AC29/Y29)</f>
+        <f t="shared" ref="AC36" si="23">(AC29/Y29)</f>
         <v>1.0215458543512672</v>
       </c>
       <c r="AD36" s="10">
-        <f t="shared" ref="AD36" si="19">(AD29/Z29)</f>
+        <f t="shared" ref="AD36" si="24">(AD29/Z29)</f>
         <v>0.9912385224811292</v>
       </c>
       <c r="AE36" s="10">
-        <f t="shared" ref="AE36" si="20">(AE29/AA29)</f>
+        <f t="shared" ref="AE36" si="25">(AE29/AA29)</f>
         <v>0.9868049305494927</v>
       </c>
       <c r="AF36" s="10">
-        <f t="shared" ref="AF36" si="21">(AF29/AB29)</f>
+        <f t="shared" ref="AF36" si="26">(AF29/AB29)</f>
         <v>0.99997293995861491</v>
       </c>
       <c r="AG36" s="10">
-        <f t="shared" ref="AG36" si="22">(AG29/AC29)</f>
+        <f t="shared" ref="AG36" si="27">(AG29/AC29)</f>
         <v>0.97512083195064214</v>
       </c>
       <c r="AH36" s="10">
-        <f t="shared" ref="AH36" si="23">(AH29/AD29)</f>
+        <f t="shared" ref="AH36" si="28">(AH29/AD29)</f>
         <v>1.0126665564943758</v>
       </c>
       <c r="AI36" s="10">
-        <f t="shared" ref="AI36" si="24">(AI29/AE29)</f>
+        <f t="shared" ref="AI36" si="29">(AI29/AE29)</f>
         <v>1.0105522135814189</v>
       </c>
       <c r="AJ36" s="10">
-        <f t="shared" ref="AJ36" si="25">(AJ29/AF29)</f>
+        <f t="shared" ref="AJ36" si="30">(AJ29/AF29)</f>
         <v>0.9286652643770601</v>
       </c>
       <c r="AK36" s="10">
-        <f t="shared" ref="AK36" si="26">(AK29/AG29)</f>
+        <f t="shared" ref="AK36" si="31">(AK29/AG29)</f>
         <v>0.93429060338161229</v>
       </c>
       <c r="AL36" s="10">
-        <f t="shared" ref="AL36" si="27">(AL29/AH29)</f>
+        <f t="shared" ref="AL36" si="32">(AL29/AH29)</f>
         <v>0.91485899518932068</v>
       </c>
       <c r="AM36" s="10">
-        <f t="shared" ref="AM36" si="28">(AM29/AI29)</f>
+        <f t="shared" ref="AM36" si="33">(AM29/AI29)</f>
         <v>0.89113832927969772</v>
       </c>
       <c r="AN36" s="10">
-        <f t="shared" ref="AN36" si="29">(AN29/AJ29)</f>
+        <f t="shared" ref="AN36" si="34">(AN29/AJ29)</f>
         <v>0.84007900197980068</v>
       </c>
       <c r="AO36" s="10">
-        <f t="shared" ref="AO36" si="30">(AO29/AK29)</f>
+        <f t="shared" ref="AO36" si="35">(AO29/AK29)</f>
         <v>0.98231801591735024</v>
       </c>
       <c r="AP36" s="10">
-        <f t="shared" ref="AP36" si="31">(AP29/AL29)</f>
+        <f t="shared" ref="AP36" si="36">(AP29/AL29)</f>
         <v>0.9863521598752949</v>
       </c>
       <c r="AQ36" s="10">
-        <f t="shared" ref="AQ36" si="32">(AQ29/AM29)</f>
+        <f t="shared" ref="AQ36" si="37">(AQ29/AM29)</f>
         <v>0.94729887059314688</v>
       </c>
       <c r="AR36" s="10">
-        <f t="shared" ref="AR36" si="33">(AR29/AN29)</f>
+        <f t="shared" ref="AR36" si="38">(AR29/AN29)</f>
         <v>1.2607689151799513</v>
       </c>
       <c r="AS36" s="10">
-        <f t="shared" ref="AS36" si="34">(AS29/AO29)</f>
+        <f t="shared" ref="AS36" si="39">(AS29/AO29)</f>
         <v>1.0572107803982338</v>
       </c>
       <c r="AT36" s="10">
-        <f t="shared" ref="AT36" si="35">(AT29/AP29)</f>
+        <f t="shared" ref="AT36" si="40">(AT29/AP29)</f>
         <v>1.0986522264414422</v>
       </c>
       <c r="AU36" s="10">
-        <f t="shared" ref="AU36" si="36">(AU29/AQ29)</f>
+        <f t="shared" ref="AU36" si="41">(AU29/AQ29)</f>
         <v>1.1741982339434403</v>
       </c>
       <c r="AV36" s="10">
-        <f t="shared" ref="AV36" si="37">(AV29/AR29)</f>
+        <f t="shared" ref="AV36" si="42">(AV29/AR29)</f>
         <v>1.0243471530406525</v>
       </c>
       <c r="AW36" s="10">
-        <f t="shared" ref="AW36" si="38">(AW29/AS29)</f>
+        <f t="shared" ref="AW36" si="43">(AW29/AS29)</f>
         <v>1.0697086755441454</v>
       </c>
       <c r="AX36" s="10">
-        <f t="shared" ref="AX36" si="39">(AX29/AT29)</f>
+        <f t="shared" ref="AX36" si="44">(AX29/AT29)</f>
         <v>1.0314243240117227</v>
       </c>
       <c r="AY36" s="10">
-        <f t="shared" ref="AY36" si="40">(AY29/AU29)</f>
+        <f t="shared" ref="AY36" si="45">(AY29/AU29)</f>
         <v>1.0311630378317829</v>
       </c>
       <c r="AZ36" s="10">
-        <f t="shared" ref="AZ36" si="41">(AZ29/AV29)</f>
+        <f t="shared" ref="AZ36" si="46">(AZ29/AV29)</f>
         <v>1.0520845559325067</v>
       </c>
       <c r="BA36" s="10">
-        <f t="shared" ref="BA36" si="42">(BA29/AW29)</f>
+        <f t="shared" ref="BA36" si="47">(BA29/AW29)</f>
         <v>1.0706508708985307</v>
       </c>
       <c r="BB36" s="10">
-        <f t="shared" ref="BB36" si="43">(BB29/AX29)</f>
+        <f t="shared" ref="BB36" si="48">(BB29/AX29)</f>
         <v>0.98334633618663725</v>
       </c>
     </row>
@@ -5183,179 +5189,179 @@
         <v>71</v>
       </c>
       <c r="K37" s="10">
-        <f t="shared" ref="K37" si="44">(K30/G30)</f>
+        <f t="shared" ref="K37" si="49">(K30/G30)</f>
         <v>1.0751285092492857</v>
       </c>
       <c r="L37" s="10">
-        <f t="shared" ref="L37" si="45">(L30/H30)</f>
+        <f t="shared" ref="L37" si="50">(L30/H30)</f>
         <v>0.99988896480277778</v>
       </c>
       <c r="M37" s="10">
-        <f t="shared" ref="M37" si="46">(M30/I30)</f>
+        <f t="shared" ref="M37" si="51">(M30/I30)</f>
         <v>1.0042974931098996</v>
       </c>
       <c r="N37" s="10">
-        <f t="shared" ref="N37" si="47">(N30/J30)</f>
+        <f t="shared" ref="N37" si="52">(N30/J30)</f>
         <v>1.0263674994192997</v>
       </c>
       <c r="O37" s="10">
-        <f t="shared" ref="O37" si="48">(O30/K30)</f>
+        <f t="shared" ref="O37" si="53">(O30/K30)</f>
         <v>1.0543785566305606</v>
       </c>
       <c r="P37" s="10">
-        <f t="shared" ref="P37" si="49">(P30/L30)</f>
+        <f t="shared" ref="P37" si="54">(P30/L30)</f>
         <v>1.0464385133711949</v>
       </c>
       <c r="Q37" s="10">
-        <f t="shared" ref="Q37" si="50">(Q30/M30)</f>
+        <f t="shared" ref="Q37" si="55">(Q30/M30)</f>
         <v>1.1108166788203855</v>
       </c>
       <c r="R37" s="10">
-        <f t="shared" ref="R37" si="51">(R30/N30)</f>
+        <f t="shared" ref="R37" si="56">(R30/N30)</f>
         <v>1.0753214390598806</v>
       </c>
       <c r="S37" s="10">
-        <f t="shared" ref="S37" si="52">(S30/O30)</f>
+        <f t="shared" ref="S37" si="57">(S30/O30)</f>
         <v>1.024534609485134</v>
       </c>
       <c r="T37" s="10">
-        <f t="shared" ref="T37" si="53">(T30/P30)</f>
+        <f t="shared" ref="T37" si="58">(T30/P30)</f>
         <v>1.0626363243598227</v>
       </c>
       <c r="U37" s="10">
-        <f t="shared" ref="U37" si="54">(U30/Q30)</f>
+        <f t="shared" ref="U37" si="59">(U30/Q30)</f>
         <v>0.99724679431484642</v>
       </c>
       <c r="V37" s="10">
-        <f t="shared" ref="V37" si="55">(V30/R30)</f>
+        <f t="shared" ref="V37" si="60">(V30/R30)</f>
         <v>0.99593316420274436</v>
       </c>
       <c r="W37" s="10">
-        <f t="shared" ref="W37" si="56">(W30/S30)</f>
+        <f t="shared" ref="W37" si="61">(W30/S30)</f>
         <v>1.0210769361276515</v>
       </c>
       <c r="X37" s="10">
-        <f t="shared" ref="X37" si="57">(X30/T30)</f>
+        <f t="shared" ref="X37" si="62">(X30/T30)</f>
         <v>1.0042855704237894</v>
       </c>
       <c r="Y37" s="10">
-        <f t="shared" ref="Y37" si="58">(Y30/U30)</f>
+        <f t="shared" ref="Y37" si="63">(Y30/U30)</f>
         <v>1.0321787478549771</v>
       </c>
       <c r="Z37" s="10">
-        <f t="shared" ref="Z37" si="59">(Z30/V30)</f>
+        <f t="shared" ref="Z37" si="64">(Z30/V30)</f>
         <v>1.0648518680367864</v>
       </c>
       <c r="AA37" s="10">
-        <f t="shared" ref="AA37" si="60">(AA30/W30)</f>
+        <f t="shared" ref="AA37" si="65">(AA30/W30)</f>
         <v>1.0624733862190625</v>
       </c>
       <c r="AB37" s="10">
-        <f t="shared" ref="AB37" si="61">(AB30/X30)</f>
+        <f t="shared" ref="AB37" si="66">(AB30/X30)</f>
         <v>1.0643079404231068</v>
       </c>
       <c r="AC37" s="10">
-        <f t="shared" ref="AC37" si="62">(AC30/Y30)</f>
+        <f t="shared" ref="AC37" si="67">(AC30/Y30)</f>
         <v>1.0558764809122887</v>
       </c>
       <c r="AD37" s="10">
-        <f t="shared" ref="AD37" si="63">(AD30/Z30)</f>
+        <f t="shared" ref="AD37" si="68">(AD30/Z30)</f>
         <v>1.0681678435528732</v>
       </c>
       <c r="AE37" s="10">
-        <f t="shared" ref="AE37" si="64">(AE30/AA30)</f>
+        <f t="shared" ref="AE37" si="69">(AE30/AA30)</f>
         <v>1.0462095323248883</v>
       </c>
       <c r="AF37" s="10">
-        <f t="shared" ref="AF37" si="65">(AF30/AB30)</f>
+        <f t="shared" ref="AF37" si="70">(AF30/AB30)</f>
         <v>1.0482329025953716</v>
       </c>
       <c r="AG37" s="10">
-        <f t="shared" ref="AG37" si="66">(AG30/AC30)</f>
+        <f t="shared" ref="AG37" si="71">(AG30/AC30)</f>
         <v>1.040245568769832</v>
       </c>
       <c r="AH37" s="10">
-        <f t="shared" ref="AH37" si="67">(AH30/AD30)</f>
+        <f t="shared" ref="AH37" si="72">(AH30/AD30)</f>
         <v>1.0189592040974371</v>
       </c>
       <c r="AI37" s="10">
-        <f t="shared" ref="AI37" si="68">(AI30/AE30)</f>
+        <f t="shared" ref="AI37" si="73">(AI30/AE30)</f>
         <v>1.00269906746167</v>
       </c>
       <c r="AJ37" s="10">
-        <f t="shared" ref="AJ37" si="69">(AJ30/AF30)</f>
+        <f t="shared" ref="AJ37" si="74">(AJ30/AF30)</f>
         <v>1.0090962298128385</v>
       </c>
       <c r="AK37" s="10">
-        <f t="shared" ref="AK37" si="70">(AK30/AG30)</f>
+        <f t="shared" ref="AK37" si="75">(AK30/AG30)</f>
         <v>0.99146215298535501</v>
       </c>
       <c r="AL37" s="10">
-        <f t="shared" ref="AL37" si="71">(AL30/AH30)</f>
+        <f t="shared" ref="AL37" si="76">(AL30/AH30)</f>
         <v>1.0165940359427574</v>
       </c>
       <c r="AM37" s="10">
-        <f t="shared" ref="AM37" si="72">(AM30/AI30)</f>
+        <f t="shared" ref="AM37" si="77">(AM30/AI30)</f>
         <v>0.96904003317694032</v>
       </c>
       <c r="AN37" s="10">
-        <f t="shared" ref="AN37" si="73">(AN30/AJ30)</f>
+        <f t="shared" ref="AN37" si="78">(AN30/AJ30)</f>
         <v>0.69401402698374104</v>
       </c>
       <c r="AO37" s="10">
-        <f t="shared" ref="AO37" si="74">(AO30/AK30)</f>
+        <f t="shared" ref="AO37" si="79">(AO30/AK30)</f>
         <v>0.85702881166432499</v>
       </c>
       <c r="AP37" s="10">
-        <f t="shared" ref="AP37" si="75">(AP30/AL30)</f>
+        <f t="shared" ref="AP37" si="80">(AP30/AL30)</f>
         <v>0.78568116465731741</v>
       </c>
       <c r="AQ37" s="10">
-        <f t="shared" ref="AQ37" si="76">(AQ30/AM30)</f>
+        <f t="shared" ref="AQ37" si="81">(AQ30/AM30)</f>
         <v>0.74956571982661402</v>
       </c>
       <c r="AR37" s="10">
-        <f t="shared" ref="AR37" si="77">(AR30/AN30)</f>
+        <f t="shared" ref="AR37" si="82">(AR30/AN30)</f>
         <v>1.2798005516502784</v>
       </c>
       <c r="AS37" s="10">
-        <f t="shared" ref="AS37" si="78">(AS30/AO30)</f>
+        <f t="shared" ref="AS37" si="83">(AS30/AO30)</f>
         <v>1.0960647813587419</v>
       </c>
       <c r="AT37" s="10">
-        <f t="shared" ref="AT37" si="79">(AT30/AP30)</f>
+        <f t="shared" ref="AT37" si="84">(AT30/AP30)</f>
         <v>1.2719737593175151</v>
       </c>
       <c r="AU37" s="10">
-        <f t="shared" ref="AU37" si="80">(AU30/AQ30)</f>
+        <f t="shared" ref="AU37" si="85">(AU30/AQ30)</f>
         <v>1.2885011373299213</v>
       </c>
       <c r="AV37" s="10">
-        <f t="shared" ref="AV37" si="81">(AV30/AR30)</f>
+        <f t="shared" ref="AV37" si="86">(AV30/AR30)</f>
         <v>1.1592923964455706</v>
       </c>
       <c r="AW37" s="10">
-        <f t="shared" ref="AW37" si="82">(AW30/AS30)</f>
+        <f t="shared" ref="AW37" si="87">(AW30/AS30)</f>
         <v>1.1634006772449141</v>
       </c>
       <c r="AX37" s="10">
-        <f t="shared" ref="AX37" si="83">(AX30/AT30)</f>
+        <f t="shared" ref="AX37" si="88">(AX30/AT30)</f>
         <v>1.0755044152407365</v>
       </c>
       <c r="AY37" s="10">
-        <f t="shared" ref="AY37" si="84">(AY30/AU30)</f>
+        <f t="shared" ref="AY37" si="89">(AY30/AU30)</f>
         <v>1.236796436185972</v>
       </c>
       <c r="AZ37" s="10">
-        <f t="shared" ref="AZ37" si="85">(AZ30/AV30)</f>
+        <f t="shared" ref="AZ37" si="90">(AZ30/AV30)</f>
         <v>1.1672996185911448</v>
       </c>
       <c r="BA37" s="10">
-        <f t="shared" ref="BA37" si="86">(BA30/AW30)</f>
+        <f t="shared" ref="BA37" si="91">(BA30/AW30)</f>
         <v>1.162151633648705</v>
       </c>
       <c r="BB37" s="10">
-        <f t="shared" ref="BB37" si="87">(BB30/AX30)</f>
+        <f t="shared" ref="BB37" si="92">(BB30/AX30)</f>
         <v>0.95315065005230692</v>
       </c>
     </row>
@@ -5438,175 +5444,175 @@
         <v>1.0727648191764818</v>
       </c>
       <c r="L42" s="10">
-        <f t="shared" ref="L42:BB47" si="88">L14/H14</f>
+        <f t="shared" ref="L42:BB47" si="93">L14/H14</f>
         <v>1.1397977185581574</v>
       </c>
       <c r="M42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1520009582739563</v>
       </c>
       <c r="N42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1715230201452058</v>
       </c>
       <c r="O42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1756113959562653</v>
       </c>
       <c r="P42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1608373866356165</v>
       </c>
       <c r="Q42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.146021242663229</v>
       </c>
       <c r="R42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1330965856122193</v>
       </c>
       <c r="S42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1529562205401047</v>
       </c>
       <c r="T42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1562056493237611</v>
       </c>
       <c r="U42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1725467848212685</v>
       </c>
       <c r="V42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1343978983990528</v>
       </c>
       <c r="W42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1259750425223303</v>
       </c>
       <c r="X42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1382282728431885</v>
       </c>
       <c r="Y42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1181068310173008</v>
       </c>
       <c r="Z42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1184406293169278</v>
       </c>
       <c r="AA42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1520606571307064</v>
       </c>
       <c r="AB42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1438419835213089</v>
       </c>
       <c r="AC42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1218715197138667</v>
       </c>
       <c r="AD42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0987024334390365</v>
       </c>
       <c r="AE42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0757294137688815</v>
       </c>
       <c r="AF42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0710010950881486</v>
       </c>
       <c r="AG42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0767377495863317</v>
       </c>
       <c r="AH42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0989070968612422</v>
       </c>
       <c r="AI42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1000817190915169</v>
       </c>
       <c r="AJ42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0724409172857547</v>
       </c>
       <c r="AK42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0714108816246122</v>
       </c>
       <c r="AL42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0658284162481058</v>
       </c>
       <c r="AM42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.90766919774459198</v>
       </c>
       <c r="AN42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.57842182125473574</v>
       </c>
       <c r="AO42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.90652149126932768</v>
       </c>
       <c r="AP42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.7770265021689452</v>
       </c>
       <c r="AQ42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.77442477940764165</v>
       </c>
       <c r="AR42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.6520064257546547</v>
       </c>
       <c r="AS42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1305041958749138</v>
       </c>
       <c r="AT42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.3173459951556687</v>
       </c>
       <c r="AU42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.4742951728457361</v>
       </c>
       <c r="AV42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1218623764035414</v>
       </c>
       <c r="AW42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.085090964839849</v>
       </c>
       <c r="AX42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.042585409674827</v>
       </c>
       <c r="AY42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1247803287230975</v>
       </c>
       <c r="AZ42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1240677340621057</v>
       </c>
       <c r="BA42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0961496537970725</v>
       </c>
       <c r="BB42" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0972641992115637</v>
       </c>
     </row>
@@ -5615,179 +5621,179 @@
         <v>60</v>
       </c>
       <c r="K43" s="10">
-        <f t="shared" ref="K43:K47" si="89">K15/G15</f>
+        <f t="shared" ref="K43:K47" si="94">K15/G15</f>
         <v>1.0059982209821259</v>
       </c>
       <c r="L43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0930944111941234</v>
       </c>
       <c r="M43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1385747263239276</v>
       </c>
       <c r="N43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1653772093469632</v>
       </c>
       <c r="O43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1416570778948494</v>
       </c>
       <c r="P43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1372794830411861</v>
       </c>
       <c r="Q43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1535795768476571</v>
       </c>
       <c r="R43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1736203684505295</v>
       </c>
       <c r="S43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2064009252206194</v>
       </c>
       <c r="T43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2635919640823563</v>
       </c>
       <c r="U43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.3047644447134259</v>
       </c>
       <c r="V43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1672085670462398</v>
       </c>
       <c r="W43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2080763262047616</v>
       </c>
       <c r="X43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1830431503229424</v>
       </c>
       <c r="Y43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1542590892145381</v>
       </c>
       <c r="Z43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1697365659349173</v>
       </c>
       <c r="AA43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1476704821034602</v>
       </c>
       <c r="AB43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1493968119397238</v>
       </c>
       <c r="AC43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.126995281949462</v>
       </c>
       <c r="AD43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1502503579233125</v>
       </c>
       <c r="AE43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1472258242597464</v>
       </c>
       <c r="AF43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1251808903396063</v>
       </c>
       <c r="AG43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1073777497287174</v>
       </c>
       <c r="AH43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1421251916604807</v>
       </c>
       <c r="AI43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1129946576594443</v>
       </c>
       <c r="AJ43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.108512755084734</v>
       </c>
       <c r="AK43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0954878655501088</v>
       </c>
       <c r="AL43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1078420257681048</v>
       </c>
       <c r="AM43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.95378545950449811</v>
       </c>
       <c r="AN43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.58283405447035674</v>
       </c>
       <c r="AO43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.92935255064925504</v>
       </c>
       <c r="AP43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.77330498402038927</v>
       </c>
       <c r="AQ43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.76898767592314143</v>
       </c>
       <c r="AR43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.6897807936581952</v>
       </c>
       <c r="AS43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1646171228276914</v>
       </c>
       <c r="AT43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.425581036178251</v>
       </c>
       <c r="AU43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.5128887031993179</v>
       </c>
       <c r="AV43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1697075833145363</v>
       </c>
       <c r="AW43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1353564372617333</v>
       </c>
       <c r="AX43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0537772124786398</v>
       </c>
       <c r="AY43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1901849431397395</v>
       </c>
       <c r="AZ43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1743981598057487</v>
       </c>
       <c r="BA43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0626267636240765</v>
       </c>
       <c r="BB43" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1335535182780978</v>
       </c>
     </row>
@@ -5796,179 +5802,179 @@
         <v>61</v>
       </c>
       <c r="K44" s="10">
-        <f t="shared" si="89"/>
+        <f t="shared" si="94"/>
         <v>0.92196844960627855</v>
       </c>
       <c r="L44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0101090687241756</v>
       </c>
       <c r="M44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0798808501840054</v>
       </c>
       <c r="N44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1206502259802102</v>
       </c>
       <c r="O44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1810419323832233</v>
       </c>
       <c r="P44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1544012366797174</v>
       </c>
       <c r="Q44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0854738557184043</v>
       </c>
       <c r="R44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1150810845821157</v>
       </c>
       <c r="S44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1154671223751358</v>
       </c>
       <c r="T44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1355675317714253</v>
       </c>
       <c r="U44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1420977361825166</v>
       </c>
       <c r="V44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.095510053151586</v>
       </c>
       <c r="W44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1692525982311768</v>
       </c>
       <c r="X44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1776790971501201</v>
       </c>
       <c r="Y44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1536963124695281</v>
       </c>
       <c r="Z44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1368770069449627</v>
       </c>
       <c r="AA44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0840334568523025</v>
       </c>
       <c r="AB44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0908460424136062</v>
       </c>
       <c r="AC44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0847326496047307</v>
       </c>
       <c r="AD44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.121277568458058</v>
       </c>
       <c r="AE44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1267624245787098</v>
       </c>
       <c r="AF44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1029448831338853</v>
       </c>
       <c r="AG44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0962249164107216</v>
       </c>
       <c r="AH44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1424736851971617</v>
       </c>
       <c r="AI44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1519727668102868</v>
       </c>
       <c r="AJ44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1252716605015436</v>
       </c>
       <c r="AK44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1307576631339038</v>
       </c>
       <c r="AL44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1180158237746318</v>
       </c>
       <c r="AM44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.96120898520445675</v>
       </c>
       <c r="AN44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.62147269978120223</v>
       </c>
       <c r="AO44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.94631164322222838</v>
       </c>
       <c r="AP44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.79692696896148763</v>
       </c>
       <c r="AQ44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.79202118671308874</v>
       </c>
       <c r="AR44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.6711527456233901</v>
       </c>
       <c r="AS44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1710766263370158</v>
       </c>
       <c r="AT44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.4093640114870425</v>
       </c>
       <c r="AU44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.4879925000385081</v>
       </c>
       <c r="AV44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.140079929487716</v>
       </c>
       <c r="AW44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1231135563236843</v>
       </c>
       <c r="AX44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.059889951713507</v>
       </c>
       <c r="AY44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1447149314837095</v>
       </c>
       <c r="AZ44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1242504661253783</v>
       </c>
       <c r="BA44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0138858173548213</v>
       </c>
       <c r="BB44" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0674936844826475</v>
       </c>
     </row>
@@ -5977,179 +5983,179 @@
         <v>62</v>
       </c>
       <c r="K45" s="10">
-        <f t="shared" si="89"/>
+        <f t="shared" si="94"/>
         <v>1.1790048297684292</v>
       </c>
       <c r="L45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2202021410050075</v>
       </c>
       <c r="M45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1654658148013204</v>
       </c>
       <c r="N45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2065492410688174</v>
       </c>
       <c r="O45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2434745440899682</v>
       </c>
       <c r="P45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2943471523340422</v>
       </c>
       <c r="Q45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2620058424766711</v>
       </c>
       <c r="R45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2007019138572541</v>
       </c>
       <c r="S45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1504205732288872</v>
       </c>
       <c r="T45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1308447436207096</v>
       </c>
       <c r="U45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1138632313879766</v>
       </c>
       <c r="V45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1531111326241512</v>
       </c>
       <c r="W45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1647861874014138</v>
       </c>
       <c r="X45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2105852971540294</v>
       </c>
       <c r="Y45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1638312418862879</v>
       </c>
       <c r="Z45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1482846772600566</v>
       </c>
       <c r="AA45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1834358031169765</v>
       </c>
       <c r="AB45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1226826600700421</v>
       </c>
       <c r="AC45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1488855511796054</v>
       </c>
       <c r="AD45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1008432234794168</v>
       </c>
       <c r="AE45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0657358550790994</v>
       </c>
       <c r="AF45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1015139479101173</v>
       </c>
       <c r="AG45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0615421063880592</v>
       </c>
       <c r="AH45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.110803931785372</v>
       </c>
       <c r="AI45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1275879683821664</v>
       </c>
       <c r="AJ45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0479767152758392</v>
       </c>
       <c r="AK45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.101084640762571</v>
       </c>
       <c r="AL45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0879174138774446</v>
       </c>
       <c r="AM45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.99238864399333959</v>
       </c>
       <c r="AN45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.81590254904676174</v>
       </c>
       <c r="AO45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.95797892925262274</v>
       </c>
       <c r="AP45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.92132959098544009</v>
       </c>
       <c r="AQ45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0022168616889089</v>
       </c>
       <c r="AR45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.3386613333768798</v>
       </c>
       <c r="AS45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.111283011615342</v>
       </c>
       <c r="AT45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1812332284732081</v>
       </c>
       <c r="AU45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1619639368380594</v>
       </c>
       <c r="AV45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0702764032237249</v>
       </c>
       <c r="AW45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0732570609340377</v>
       </c>
       <c r="AX45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.97074301358998749</v>
       </c>
       <c r="AY45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0709855748418096</v>
       </c>
       <c r="AZ45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0730976759080224</v>
       </c>
       <c r="BA45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0298950547875421</v>
       </c>
       <c r="BB45" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1220592837373575</v>
       </c>
     </row>
@@ -6158,179 +6164,179 @@
         <v>63</v>
       </c>
       <c r="K46" s="10">
-        <f t="shared" si="89"/>
+        <f t="shared" si="94"/>
         <v>0.99347416959906731</v>
       </c>
       <c r="L46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0842147941297187</v>
       </c>
       <c r="M46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0662625799538052</v>
       </c>
       <c r="N46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0937804512575158</v>
       </c>
       <c r="O46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1741608551855647</v>
       </c>
       <c r="P46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1770827313289833</v>
       </c>
       <c r="Q46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2341951436365808</v>
       </c>
       <c r="R46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2479324212937759</v>
       </c>
       <c r="S46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2504885969982653</v>
       </c>
       <c r="T46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2822470911358204</v>
       </c>
       <c r="U46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2738516911049309</v>
       </c>
       <c r="V46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2056699644542999</v>
       </c>
       <c r="W46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1571355116626916</v>
       </c>
       <c r="X46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1563545158080575</v>
       </c>
       <c r="Y46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.115028534612347</v>
       </c>
       <c r="Z46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1291494898916945</v>
       </c>
       <c r="AA46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.178720635414455</v>
       </c>
       <c r="AB46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1516388147537415</v>
       </c>
       <c r="AC46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1333571414720305</v>
       </c>
       <c r="AD46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1617353151680232</v>
       </c>
       <c r="AE46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.166403651067204</v>
       </c>
       <c r="AF46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.148138762391629</v>
       </c>
       <c r="AG46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1163602589405934</v>
       </c>
       <c r="AH46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1731577727210549</v>
       </c>
       <c r="AI46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1341308404245303</v>
       </c>
       <c r="AJ46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0973808352433976</v>
       </c>
       <c r="AK46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1465629732008598</v>
       </c>
       <c r="AL46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1244576054390572</v>
       </c>
       <c r="AM46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0554191485099624</v>
       </c>
       <c r="AN46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.76954473394927214</v>
       </c>
       <c r="AO46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.97163317371178914</v>
       </c>
       <c r="AP46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.92502222892620645</v>
       </c>
       <c r="AQ46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.9575921673074379</v>
       </c>
       <c r="AR46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.4227708321884631</v>
       </c>
       <c r="AS46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1135946050787082</v>
       </c>
       <c r="AT46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.22696856719712</v>
       </c>
       <c r="AU46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2083930324171448</v>
       </c>
       <c r="AV46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0889000291357425</v>
       </c>
       <c r="AW46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1069688918009883</v>
       </c>
       <c r="AX46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.032605536756283</v>
       </c>
       <c r="AY46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0874664384908421</v>
       </c>
       <c r="AZ46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.085857522312843</v>
       </c>
       <c r="BA46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0535049730328669</v>
       </c>
       <c r="BB46" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0855390815751704</v>
       </c>
     </row>
@@ -6339,183 +6345,196 @@
         <v>64</v>
       </c>
       <c r="K47" s="10">
-        <f t="shared" si="89"/>
+        <f t="shared" si="94"/>
         <v>1.0504004342561277</v>
       </c>
       <c r="L47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0273769100169781</v>
       </c>
       <c r="M47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1065627522195316</v>
       </c>
       <c r="N47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1746170904027646</v>
       </c>
       <c r="O47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0303381083297158</v>
       </c>
       <c r="P47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1809801693864901</v>
       </c>
       <c r="Q47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0430788867868619</v>
       </c>
       <c r="R47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0686657593186106</v>
       </c>
       <c r="S47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.182660799550604</v>
       </c>
       <c r="T47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1744102149244593</v>
       </c>
       <c r="U47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2032864978257547</v>
       </c>
       <c r="V47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1624419703381128</v>
       </c>
       <c r="W47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1511972036829541</v>
       </c>
       <c r="X47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2005622370331757</v>
       </c>
       <c r="Y47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1513638179638979</v>
       </c>
       <c r="Z47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.118801908464393</v>
       </c>
       <c r="AA47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1197624904123356</v>
       </c>
       <c r="AB47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0815823344239923</v>
       </c>
       <c r="AC47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1579785807794829</v>
       </c>
       <c r="AD47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1984268633613953</v>
       </c>
       <c r="AE47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1374857985076918</v>
       </c>
       <c r="AF47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1608361530079716</v>
       </c>
       <c r="AG47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.110097116471662</v>
       </c>
       <c r="AH47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1694079814434075</v>
       </c>
       <c r="AI47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2171307481542468</v>
       </c>
       <c r="AJ47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.2088036953783068</v>
       </c>
       <c r="AK47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1679877300613497</v>
       </c>
       <c r="AL47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.1912769074721064</v>
       </c>
       <c r="AM47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0577118055826362</v>
       </c>
       <c r="AN47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.75245218244237388</v>
       </c>
       <c r="AO47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0222079818470236</v>
       </c>
       <c r="AP47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.921269228586025</v>
       </c>
       <c r="AQ47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.96404684547675012</v>
       </c>
       <c r="AR47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.6403644560317201</v>
       </c>
       <c r="AS47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.288258568418889</v>
       </c>
       <c r="AT47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.3544362292051753</v>
       </c>
       <c r="AU47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.3138410675250947</v>
       </c>
       <c r="AV47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0165310464144102</v>
       </c>
       <c r="AW47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0199514973594779</v>
       </c>
       <c r="AX47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>0.99851396944539228</v>
       </c>
       <c r="AY47" s="10">
-        <f t="shared" si="88"/>
+        <f t="shared" si="93"/>
         <v>1.0956302924450996</v>
       </c>
       <c r="AZ47" s="10">
-        <f t="shared" ref="AZ47" si="90">AZ19/AV19</f>
+        <f t="shared" ref="AZ47" si="95">AZ19/AV19</f>
         <v>1.1066612377850167</v>
       </c>
       <c r="BA47" s="10">
-        <f t="shared" ref="BA47" si="91">BA19/AW19</f>
+        <f t="shared" ref="BA47" si="96">BA19/AW19</f>
         <v>1.031261976457706</v>
       </c>
       <c r="BB47" s="10">
-        <f t="shared" ref="BB47" si="92">BB19/AX19</f>
+        <f t="shared" ref="BB47" si="97">BB19/AX19</f>
         <v>0.9933864342174199</v>
+      </c>
+    </row>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G50" t="s">
+        <v>74</v>
+      </c>
+      <c r="H50" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H50" xr:uid="{4D480346-D891-4739-8DAD-77B94267578F}">
+      <formula1>$J$50:$L$50</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup paperSize="9" scale="57" orientation="portrait"/>
   <headerFooter>

</xml_diff>